<commit_message>
API test design & usability test design
</commit_message>
<xml_diff>
--- a/docs/tests/test case/TestCase_CartManagement.xlsx
+++ b/docs/tests/test case/TestCase_CartManagement.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\KiemThuPhanMem_TaiLieu\Tất Cả file đồ án cuối kỳ\TestCase\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\KiemThuPhanMem_Web\fullstack-vitejs-books\docs\tests\test case\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74A60EF4-EDCD-4262-ABAA-CD3B74482B0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B68B21C-F251-483B-AB36-4465B6497009}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="3" r:id="rId1"/>
@@ -1178,28 +1178,10 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1209,13 +1191,31 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1436,7 +1436,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{985883BD-2016-4721-B27B-C0B0A9BF8844}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B6" zoomScale="85" workbookViewId="0">
+    <sheetView topLeftCell="B6" zoomScale="85" workbookViewId="0">
       <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
@@ -29529,11 +29529,11 @@
   </sheetPr>
   <dimension ref="A1:Z968"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="L59" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="J14" sqref="J14:L19"/>
+      <selection pane="bottomRight" activeCell="B2" sqref="B2:C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -29559,29 +29559,29 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="60" t="s">
+      <c r="B1" s="54" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="51"/>
-      <c r="D1" s="60" t="s">
+      <c r="C1" s="48"/>
+      <c r="D1" s="54" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="51"/>
-      <c r="F1" s="51"/>
-      <c r="G1" s="60" t="s">
+      <c r="E1" s="48"/>
+      <c r="F1" s="48"/>
+      <c r="G1" s="54" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="51"/>
-      <c r="I1" s="51"/>
-      <c r="J1" s="60" t="s">
+      <c r="H1" s="48"/>
+      <c r="I1" s="48"/>
+      <c r="J1" s="54" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="51"/>
-      <c r="L1" s="51"/>
-      <c r="M1" s="60" t="s">
+      <c r="K1" s="48"/>
+      <c r="L1" s="48"/>
+      <c r="M1" s="54" t="s">
         <v>5</v>
       </c>
-      <c r="N1" s="51"/>
+      <c r="N1" s="48"/>
       <c r="O1" s="1" t="s">
         <v>6</v>
       </c>
@@ -29602,39 +29602,39 @@
       <c r="Z1" s="3"/>
     </row>
     <row r="2" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="58" t="s">
+      <c r="A2" s="47" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="59" t="s">
+      <c r="B2" s="55" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="51"/>
-      <c r="D2" s="56" t="s">
+      <c r="C2" s="48"/>
+      <c r="D2" s="50" t="s">
         <v>60</v>
       </c>
-      <c r="E2" s="57"/>
-      <c r="F2" s="57"/>
-      <c r="G2" s="47" t="s">
+      <c r="E2" s="51"/>
+      <c r="F2" s="51"/>
+      <c r="G2" s="56" t="s">
         <v>11</v>
       </c>
-      <c r="H2" s="51"/>
-      <c r="I2" s="51"/>
-      <c r="J2" s="48" t="s">
+      <c r="H2" s="48"/>
+      <c r="I2" s="48"/>
+      <c r="J2" s="57" t="s">
         <v>12</v>
       </c>
-      <c r="K2" s="51"/>
-      <c r="L2" s="51"/>
-      <c r="M2" s="47" t="s">
+      <c r="K2" s="48"/>
+      <c r="L2" s="48"/>
+      <c r="M2" s="56" t="s">
         <v>13</v>
       </c>
-      <c r="N2" s="51"/>
-      <c r="O2" s="47" t="s">
+      <c r="N2" s="48"/>
+      <c r="O2" s="56" t="s">
         <v>13</v>
       </c>
-      <c r="P2" s="49" t="s">
+      <c r="P2" s="59" t="s">
         <v>66</v>
       </c>
-      <c r="Q2" s="50"/>
+      <c r="Q2" s="60"/>
       <c r="R2" s="3"/>
       <c r="S2" s="3"/>
       <c r="T2" s="3"/>
@@ -29646,23 +29646,23 @@
       <c r="Z2" s="3"/>
     </row>
     <row r="3" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="51"/>
-      <c r="B3" s="51"/>
-      <c r="C3" s="51"/>
-      <c r="D3" s="57"/>
-      <c r="E3" s="57"/>
-      <c r="F3" s="57"/>
-      <c r="G3" s="51"/>
-      <c r="H3" s="51"/>
-      <c r="I3" s="51"/>
-      <c r="J3" s="51"/>
-      <c r="K3" s="51"/>
-      <c r="L3" s="51"/>
-      <c r="M3" s="51"/>
-      <c r="N3" s="51"/>
-      <c r="O3" s="48"/>
-      <c r="P3" s="49"/>
-      <c r="Q3" s="50"/>
+      <c r="A3" s="48"/>
+      <c r="B3" s="48"/>
+      <c r="C3" s="48"/>
+      <c r="D3" s="51"/>
+      <c r="E3" s="51"/>
+      <c r="F3" s="51"/>
+      <c r="G3" s="48"/>
+      <c r="H3" s="48"/>
+      <c r="I3" s="48"/>
+      <c r="J3" s="48"/>
+      <c r="K3" s="48"/>
+      <c r="L3" s="48"/>
+      <c r="M3" s="48"/>
+      <c r="N3" s="48"/>
+      <c r="O3" s="57"/>
+      <c r="P3" s="59"/>
+      <c r="Q3" s="60"/>
       <c r="R3" s="3"/>
       <c r="S3" s="3"/>
       <c r="T3" s="3"/>
@@ -29674,23 +29674,23 @@
       <c r="Z3" s="3"/>
     </row>
     <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="51"/>
-      <c r="B4" s="51"/>
-      <c r="C4" s="51"/>
-      <c r="D4" s="57"/>
-      <c r="E4" s="57"/>
-      <c r="F4" s="57"/>
-      <c r="G4" s="51"/>
-      <c r="H4" s="51"/>
-      <c r="I4" s="51"/>
-      <c r="J4" s="51"/>
-      <c r="K4" s="51"/>
-      <c r="L4" s="51"/>
-      <c r="M4" s="51"/>
-      <c r="N4" s="51"/>
-      <c r="O4" s="48"/>
-      <c r="P4" s="49"/>
-      <c r="Q4" s="50"/>
+      <c r="A4" s="48"/>
+      <c r="B4" s="48"/>
+      <c r="C4" s="48"/>
+      <c r="D4" s="51"/>
+      <c r="E4" s="51"/>
+      <c r="F4" s="51"/>
+      <c r="G4" s="48"/>
+      <c r="H4" s="48"/>
+      <c r="I4" s="48"/>
+      <c r="J4" s="48"/>
+      <c r="K4" s="48"/>
+      <c r="L4" s="48"/>
+      <c r="M4" s="48"/>
+      <c r="N4" s="48"/>
+      <c r="O4" s="57"/>
+      <c r="P4" s="59"/>
+      <c r="Q4" s="60"/>
       <c r="R4" s="3"/>
       <c r="S4" s="3"/>
       <c r="T4" s="3"/>
@@ -29702,23 +29702,23 @@
       <c r="Z4" s="3"/>
     </row>
     <row r="5" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="51"/>
-      <c r="B5" s="51"/>
-      <c r="C5" s="51"/>
-      <c r="D5" s="57"/>
-      <c r="E5" s="57"/>
-      <c r="F5" s="57"/>
-      <c r="G5" s="51"/>
-      <c r="H5" s="51"/>
-      <c r="I5" s="51"/>
-      <c r="J5" s="51"/>
-      <c r="K5" s="51"/>
-      <c r="L5" s="51"/>
-      <c r="M5" s="51"/>
-      <c r="N5" s="51"/>
-      <c r="O5" s="48"/>
-      <c r="P5" s="49"/>
-      <c r="Q5" s="50"/>
+      <c r="A5" s="48"/>
+      <c r="B5" s="48"/>
+      <c r="C5" s="48"/>
+      <c r="D5" s="51"/>
+      <c r="E5" s="51"/>
+      <c r="F5" s="51"/>
+      <c r="G5" s="48"/>
+      <c r="H5" s="48"/>
+      <c r="I5" s="48"/>
+      <c r="J5" s="48"/>
+      <c r="K5" s="48"/>
+      <c r="L5" s="48"/>
+      <c r="M5" s="48"/>
+      <c r="N5" s="48"/>
+      <c r="O5" s="57"/>
+      <c r="P5" s="59"/>
+      <c r="Q5" s="60"/>
       <c r="R5" s="3"/>
       <c r="S5" s="3"/>
       <c r="T5" s="3"/>
@@ -29730,23 +29730,23 @@
       <c r="Z5" s="3"/>
     </row>
     <row r="6" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="51"/>
-      <c r="B6" s="51"/>
-      <c r="C6" s="51"/>
-      <c r="D6" s="57"/>
-      <c r="E6" s="57"/>
-      <c r="F6" s="57"/>
-      <c r="G6" s="51"/>
-      <c r="H6" s="51"/>
-      <c r="I6" s="51"/>
-      <c r="J6" s="51"/>
-      <c r="K6" s="51"/>
-      <c r="L6" s="51"/>
-      <c r="M6" s="51"/>
-      <c r="N6" s="51"/>
-      <c r="O6" s="48"/>
-      <c r="P6" s="49"/>
-      <c r="Q6" s="50"/>
+      <c r="A6" s="48"/>
+      <c r="B6" s="48"/>
+      <c r="C6" s="48"/>
+      <c r="D6" s="51"/>
+      <c r="E6" s="51"/>
+      <c r="F6" s="51"/>
+      <c r="G6" s="48"/>
+      <c r="H6" s="48"/>
+      <c r="I6" s="48"/>
+      <c r="J6" s="48"/>
+      <c r="K6" s="48"/>
+      <c r="L6" s="48"/>
+      <c r="M6" s="48"/>
+      <c r="N6" s="48"/>
+      <c r="O6" s="57"/>
+      <c r="P6" s="59"/>
+      <c r="Q6" s="60"/>
       <c r="R6" s="3"/>
       <c r="S6" s="3"/>
       <c r="T6" s="3"/>
@@ -29758,23 +29758,23 @@
       <c r="Z6" s="3"/>
     </row>
     <row r="7" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="51"/>
-      <c r="B7" s="51"/>
-      <c r="C7" s="51"/>
-      <c r="D7" s="57"/>
-      <c r="E7" s="57"/>
-      <c r="F7" s="57"/>
-      <c r="G7" s="51"/>
-      <c r="H7" s="51"/>
-      <c r="I7" s="51"/>
-      <c r="J7" s="51"/>
-      <c r="K7" s="51"/>
-      <c r="L7" s="51"/>
-      <c r="M7" s="51"/>
-      <c r="N7" s="51"/>
-      <c r="O7" s="48"/>
-      <c r="P7" s="49"/>
-      <c r="Q7" s="50"/>
+      <c r="A7" s="48"/>
+      <c r="B7" s="48"/>
+      <c r="C7" s="48"/>
+      <c r="D7" s="51"/>
+      <c r="E7" s="51"/>
+      <c r="F7" s="51"/>
+      <c r="G7" s="48"/>
+      <c r="H7" s="48"/>
+      <c r="I7" s="48"/>
+      <c r="J7" s="48"/>
+      <c r="K7" s="48"/>
+      <c r="L7" s="48"/>
+      <c r="M7" s="48"/>
+      <c r="N7" s="48"/>
+      <c r="O7" s="57"/>
+      <c r="P7" s="59"/>
+      <c r="Q7" s="60"/>
       <c r="R7" s="3"/>
       <c r="S7" s="3"/>
       <c r="T7" s="3"/>
@@ -29786,39 +29786,39 @@
       <c r="Z7" s="3"/>
     </row>
     <row r="8" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="58" t="s">
+      <c r="A8" s="47" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="55" t="s">
+      <c r="B8" s="49" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="51"/>
-      <c r="D8" s="56" t="s">
+      <c r="C8" s="48"/>
+      <c r="D8" s="50" t="s">
         <v>61</v>
       </c>
-      <c r="E8" s="57"/>
-      <c r="F8" s="57"/>
-      <c r="G8" s="54" t="s">
+      <c r="E8" s="51"/>
+      <c r="F8" s="51"/>
+      <c r="G8" s="53" t="s">
         <v>16</v>
       </c>
-      <c r="H8" s="51"/>
-      <c r="I8" s="51"/>
-      <c r="J8" s="53" t="s">
+      <c r="H8" s="48"/>
+      <c r="I8" s="48"/>
+      <c r="J8" s="52" t="s">
         <v>12</v>
       </c>
-      <c r="K8" s="51"/>
-      <c r="L8" s="51"/>
-      <c r="M8" s="54" t="s">
+      <c r="K8" s="48"/>
+      <c r="L8" s="48"/>
+      <c r="M8" s="53" t="s">
         <v>62</v>
       </c>
-      <c r="N8" s="51"/>
-      <c r="O8" s="48" t="s">
+      <c r="N8" s="48"/>
+      <c r="O8" s="57" t="s">
         <v>62</v>
       </c>
-      <c r="P8" s="49" t="s">
+      <c r="P8" s="59" t="s">
         <v>66</v>
       </c>
-      <c r="Q8" s="50"/>
+      <c r="Q8" s="60"/>
       <c r="R8" s="3"/>
       <c r="S8" s="3"/>
       <c r="T8" s="3"/>
@@ -29830,23 +29830,23 @@
       <c r="Z8" s="3"/>
     </row>
     <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="51"/>
-      <c r="B9" s="51"/>
-      <c r="C9" s="51"/>
-      <c r="D9" s="57"/>
-      <c r="E9" s="57"/>
-      <c r="F9" s="57"/>
-      <c r="G9" s="51"/>
-      <c r="H9" s="51"/>
-      <c r="I9" s="51"/>
-      <c r="J9" s="51"/>
-      <c r="K9" s="51"/>
-      <c r="L9" s="51"/>
-      <c r="M9" s="51"/>
-      <c r="N9" s="51"/>
-      <c r="O9" s="48"/>
-      <c r="P9" s="49"/>
-      <c r="Q9" s="50"/>
+      <c r="A9" s="48"/>
+      <c r="B9" s="48"/>
+      <c r="C9" s="48"/>
+      <c r="D9" s="51"/>
+      <c r="E9" s="51"/>
+      <c r="F9" s="51"/>
+      <c r="G9" s="48"/>
+      <c r="H9" s="48"/>
+      <c r="I9" s="48"/>
+      <c r="J9" s="48"/>
+      <c r="K9" s="48"/>
+      <c r="L9" s="48"/>
+      <c r="M9" s="48"/>
+      <c r="N9" s="48"/>
+      <c r="O9" s="57"/>
+      <c r="P9" s="59"/>
+      <c r="Q9" s="60"/>
       <c r="R9" s="3"/>
       <c r="S9" s="3"/>
       <c r="T9" s="3"/>
@@ -29858,23 +29858,23 @@
       <c r="Z9" s="3"/>
     </row>
     <row r="10" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="51"/>
-      <c r="B10" s="51"/>
-      <c r="C10" s="51"/>
-      <c r="D10" s="57"/>
-      <c r="E10" s="57"/>
-      <c r="F10" s="57"/>
-      <c r="G10" s="51"/>
-      <c r="H10" s="51"/>
-      <c r="I10" s="51"/>
-      <c r="J10" s="51"/>
-      <c r="K10" s="51"/>
-      <c r="L10" s="51"/>
-      <c r="M10" s="51"/>
-      <c r="N10" s="51"/>
-      <c r="O10" s="48"/>
-      <c r="P10" s="49"/>
-      <c r="Q10" s="50"/>
+      <c r="A10" s="48"/>
+      <c r="B10" s="48"/>
+      <c r="C10" s="48"/>
+      <c r="D10" s="51"/>
+      <c r="E10" s="51"/>
+      <c r="F10" s="51"/>
+      <c r="G10" s="48"/>
+      <c r="H10" s="48"/>
+      <c r="I10" s="48"/>
+      <c r="J10" s="48"/>
+      <c r="K10" s="48"/>
+      <c r="L10" s="48"/>
+      <c r="M10" s="48"/>
+      <c r="N10" s="48"/>
+      <c r="O10" s="57"/>
+      <c r="P10" s="59"/>
+      <c r="Q10" s="60"/>
       <c r="R10" s="3"/>
       <c r="S10" s="3"/>
       <c r="T10" s="3"/>
@@ -29886,23 +29886,23 @@
       <c r="Z10" s="3"/>
     </row>
     <row r="11" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="51"/>
-      <c r="B11" s="51"/>
-      <c r="C11" s="51"/>
-      <c r="D11" s="57"/>
-      <c r="E11" s="57"/>
-      <c r="F11" s="57"/>
-      <c r="G11" s="51"/>
-      <c r="H11" s="51"/>
-      <c r="I11" s="51"/>
-      <c r="J11" s="51"/>
-      <c r="K11" s="51"/>
-      <c r="L11" s="51"/>
-      <c r="M11" s="51"/>
-      <c r="N11" s="51"/>
-      <c r="O11" s="48"/>
-      <c r="P11" s="49"/>
-      <c r="Q11" s="50"/>
+      <c r="A11" s="48"/>
+      <c r="B11" s="48"/>
+      <c r="C11" s="48"/>
+      <c r="D11" s="51"/>
+      <c r="E11" s="51"/>
+      <c r="F11" s="51"/>
+      <c r="G11" s="48"/>
+      <c r="H11" s="48"/>
+      <c r="I11" s="48"/>
+      <c r="J11" s="48"/>
+      <c r="K11" s="48"/>
+      <c r="L11" s="48"/>
+      <c r="M11" s="48"/>
+      <c r="N11" s="48"/>
+      <c r="O11" s="57"/>
+      <c r="P11" s="59"/>
+      <c r="Q11" s="60"/>
       <c r="R11" s="3"/>
       <c r="S11" s="3"/>
       <c r="T11" s="3"/>
@@ -29914,23 +29914,23 @@
       <c r="Z11" s="3"/>
     </row>
     <row r="12" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="51"/>
-      <c r="B12" s="51"/>
-      <c r="C12" s="51"/>
-      <c r="D12" s="57"/>
-      <c r="E12" s="57"/>
-      <c r="F12" s="57"/>
-      <c r="G12" s="51"/>
-      <c r="H12" s="51"/>
-      <c r="I12" s="51"/>
-      <c r="J12" s="51"/>
-      <c r="K12" s="51"/>
-      <c r="L12" s="51"/>
-      <c r="M12" s="51"/>
-      <c r="N12" s="51"/>
-      <c r="O12" s="48"/>
-      <c r="P12" s="49"/>
-      <c r="Q12" s="50"/>
+      <c r="A12" s="48"/>
+      <c r="B12" s="48"/>
+      <c r="C12" s="48"/>
+      <c r="D12" s="51"/>
+      <c r="E12" s="51"/>
+      <c r="F12" s="51"/>
+      <c r="G12" s="48"/>
+      <c r="H12" s="48"/>
+      <c r="I12" s="48"/>
+      <c r="J12" s="48"/>
+      <c r="K12" s="48"/>
+      <c r="L12" s="48"/>
+      <c r="M12" s="48"/>
+      <c r="N12" s="48"/>
+      <c r="O12" s="57"/>
+      <c r="P12" s="59"/>
+      <c r="Q12" s="60"/>
       <c r="R12" s="3"/>
       <c r="S12" s="3"/>
       <c r="T12" s="3"/>
@@ -29942,23 +29942,23 @@
       <c r="Z12" s="3"/>
     </row>
     <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="51"/>
-      <c r="B13" s="51"/>
-      <c r="C13" s="51"/>
-      <c r="D13" s="57"/>
-      <c r="E13" s="57"/>
-      <c r="F13" s="57"/>
-      <c r="G13" s="51"/>
-      <c r="H13" s="51"/>
-      <c r="I13" s="51"/>
-      <c r="J13" s="51"/>
-      <c r="K13" s="51"/>
-      <c r="L13" s="51"/>
-      <c r="M13" s="51"/>
-      <c r="N13" s="51"/>
-      <c r="O13" s="48"/>
-      <c r="P13" s="49"/>
-      <c r="Q13" s="50"/>
+      <c r="A13" s="48"/>
+      <c r="B13" s="48"/>
+      <c r="C13" s="48"/>
+      <c r="D13" s="51"/>
+      <c r="E13" s="51"/>
+      <c r="F13" s="51"/>
+      <c r="G13" s="48"/>
+      <c r="H13" s="48"/>
+      <c r="I13" s="48"/>
+      <c r="J13" s="48"/>
+      <c r="K13" s="48"/>
+      <c r="L13" s="48"/>
+      <c r="M13" s="48"/>
+      <c r="N13" s="48"/>
+      <c r="O13" s="57"/>
+      <c r="P13" s="59"/>
+      <c r="Q13" s="60"/>
       <c r="R13" s="3"/>
       <c r="S13" s="3"/>
       <c r="T13" s="3"/>
@@ -29970,39 +29970,39 @@
       <c r="Z13" s="3"/>
     </row>
     <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="58" t="s">
+      <c r="A14" s="47" t="s">
         <v>17</v>
       </c>
-      <c r="B14" s="53" t="s">
+      <c r="B14" s="52" t="s">
         <v>18</v>
       </c>
-      <c r="C14" s="51"/>
-      <c r="D14" s="56" t="s">
+      <c r="C14" s="48"/>
+      <c r="D14" s="50" t="s">
         <v>63</v>
       </c>
-      <c r="E14" s="57"/>
-      <c r="F14" s="57"/>
-      <c r="G14" s="53" t="s">
+      <c r="E14" s="51"/>
+      <c r="F14" s="51"/>
+      <c r="G14" s="52" t="s">
         <v>19</v>
       </c>
-      <c r="H14" s="51"/>
-      <c r="I14" s="51"/>
-      <c r="J14" s="48" t="s">
+      <c r="H14" s="48"/>
+      <c r="I14" s="48"/>
+      <c r="J14" s="57" t="s">
         <v>20</v>
       </c>
-      <c r="K14" s="52"/>
-      <c r="L14" s="52"/>
-      <c r="M14" s="54" t="s">
+      <c r="K14" s="58"/>
+      <c r="L14" s="58"/>
+      <c r="M14" s="53" t="s">
         <v>21</v>
       </c>
-      <c r="N14" s="51"/>
-      <c r="O14" s="47" t="s">
+      <c r="N14" s="48"/>
+      <c r="O14" s="56" t="s">
         <v>21</v>
       </c>
-      <c r="P14" s="49" t="s">
+      <c r="P14" s="59" t="s">
         <v>66</v>
       </c>
-      <c r="Q14" s="50"/>
+      <c r="Q14" s="60"/>
       <c r="R14" s="3"/>
       <c r="S14" s="3"/>
       <c r="T14" s="3"/>
@@ -30014,23 +30014,23 @@
       <c r="Z14" s="3"/>
     </row>
     <row r="15" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="51"/>
-      <c r="B15" s="51"/>
-      <c r="C15" s="51"/>
-      <c r="D15" s="57"/>
-      <c r="E15" s="57"/>
-      <c r="F15" s="57"/>
-      <c r="G15" s="51"/>
-      <c r="H15" s="51"/>
-      <c r="I15" s="51"/>
-      <c r="J15" s="52"/>
-      <c r="K15" s="52"/>
-      <c r="L15" s="52"/>
-      <c r="M15" s="51"/>
-      <c r="N15" s="51"/>
-      <c r="O15" s="48"/>
-      <c r="P15" s="49"/>
-      <c r="Q15" s="50"/>
+      <c r="A15" s="48"/>
+      <c r="B15" s="48"/>
+      <c r="C15" s="48"/>
+      <c r="D15" s="51"/>
+      <c r="E15" s="51"/>
+      <c r="F15" s="51"/>
+      <c r="G15" s="48"/>
+      <c r="H15" s="48"/>
+      <c r="I15" s="48"/>
+      <c r="J15" s="58"/>
+      <c r="K15" s="58"/>
+      <c r="L15" s="58"/>
+      <c r="M15" s="48"/>
+      <c r="N15" s="48"/>
+      <c r="O15" s="57"/>
+      <c r="P15" s="59"/>
+      <c r="Q15" s="60"/>
       <c r="R15" s="3"/>
       <c r="S15" s="3"/>
       <c r="T15" s="3"/>
@@ -30042,23 +30042,23 @@
       <c r="Z15" s="3"/>
     </row>
     <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="51"/>
-      <c r="B16" s="51"/>
-      <c r="C16" s="51"/>
-      <c r="D16" s="57"/>
-      <c r="E16" s="57"/>
-      <c r="F16" s="57"/>
-      <c r="G16" s="51"/>
-      <c r="H16" s="51"/>
-      <c r="I16" s="51"/>
-      <c r="J16" s="52"/>
-      <c r="K16" s="52"/>
-      <c r="L16" s="52"/>
-      <c r="M16" s="51"/>
-      <c r="N16" s="51"/>
-      <c r="O16" s="48"/>
-      <c r="P16" s="49"/>
-      <c r="Q16" s="50"/>
+      <c r="A16" s="48"/>
+      <c r="B16" s="48"/>
+      <c r="C16" s="48"/>
+      <c r="D16" s="51"/>
+      <c r="E16" s="51"/>
+      <c r="F16" s="51"/>
+      <c r="G16" s="48"/>
+      <c r="H16" s="48"/>
+      <c r="I16" s="48"/>
+      <c r="J16" s="58"/>
+      <c r="K16" s="58"/>
+      <c r="L16" s="58"/>
+      <c r="M16" s="48"/>
+      <c r="N16" s="48"/>
+      <c r="O16" s="57"/>
+      <c r="P16" s="59"/>
+      <c r="Q16" s="60"/>
       <c r="R16" s="3"/>
       <c r="S16" s="3"/>
       <c r="T16" s="3"/>
@@ -30070,23 +30070,23 @@
       <c r="Z16" s="3"/>
     </row>
     <row r="17" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="51"/>
-      <c r="B17" s="51"/>
-      <c r="C17" s="51"/>
-      <c r="D17" s="57"/>
-      <c r="E17" s="57"/>
-      <c r="F17" s="57"/>
-      <c r="G17" s="51"/>
-      <c r="H17" s="51"/>
-      <c r="I17" s="51"/>
-      <c r="J17" s="52"/>
-      <c r="K17" s="52"/>
-      <c r="L17" s="52"/>
-      <c r="M17" s="51"/>
-      <c r="N17" s="51"/>
-      <c r="O17" s="48"/>
-      <c r="P17" s="49"/>
-      <c r="Q17" s="50"/>
+      <c r="A17" s="48"/>
+      <c r="B17" s="48"/>
+      <c r="C17" s="48"/>
+      <c r="D17" s="51"/>
+      <c r="E17" s="51"/>
+      <c r="F17" s="51"/>
+      <c r="G17" s="48"/>
+      <c r="H17" s="48"/>
+      <c r="I17" s="48"/>
+      <c r="J17" s="58"/>
+      <c r="K17" s="58"/>
+      <c r="L17" s="58"/>
+      <c r="M17" s="48"/>
+      <c r="N17" s="48"/>
+      <c r="O17" s="57"/>
+      <c r="P17" s="59"/>
+      <c r="Q17" s="60"/>
       <c r="R17" s="3"/>
       <c r="S17" s="3"/>
       <c r="T17" s="3"/>
@@ -30098,23 +30098,23 @@
       <c r="Z17" s="3"/>
     </row>
     <row r="18" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="51"/>
-      <c r="B18" s="51"/>
-      <c r="C18" s="51"/>
-      <c r="D18" s="57"/>
-      <c r="E18" s="57"/>
-      <c r="F18" s="57"/>
-      <c r="G18" s="51"/>
-      <c r="H18" s="51"/>
-      <c r="I18" s="51"/>
-      <c r="J18" s="52"/>
-      <c r="K18" s="52"/>
-      <c r="L18" s="52"/>
-      <c r="M18" s="51"/>
-      <c r="N18" s="51"/>
-      <c r="O18" s="48"/>
-      <c r="P18" s="49"/>
-      <c r="Q18" s="50"/>
+      <c r="A18" s="48"/>
+      <c r="B18" s="48"/>
+      <c r="C18" s="48"/>
+      <c r="D18" s="51"/>
+      <c r="E18" s="51"/>
+      <c r="F18" s="51"/>
+      <c r="G18" s="48"/>
+      <c r="H18" s="48"/>
+      <c r="I18" s="48"/>
+      <c r="J18" s="58"/>
+      <c r="K18" s="58"/>
+      <c r="L18" s="58"/>
+      <c r="M18" s="48"/>
+      <c r="N18" s="48"/>
+      <c r="O18" s="57"/>
+      <c r="P18" s="59"/>
+      <c r="Q18" s="60"/>
       <c r="R18" s="3"/>
       <c r="S18" s="3"/>
       <c r="T18" s="3"/>
@@ -30126,23 +30126,23 @@
       <c r="Z18" s="3"/>
     </row>
     <row r="19" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="51"/>
-      <c r="B19" s="51"/>
-      <c r="C19" s="51"/>
-      <c r="D19" s="57"/>
-      <c r="E19" s="57"/>
-      <c r="F19" s="57"/>
-      <c r="G19" s="51"/>
-      <c r="H19" s="51"/>
-      <c r="I19" s="51"/>
-      <c r="J19" s="52"/>
-      <c r="K19" s="52"/>
-      <c r="L19" s="52"/>
-      <c r="M19" s="51"/>
-      <c r="N19" s="51"/>
-      <c r="O19" s="48"/>
-      <c r="P19" s="49"/>
-      <c r="Q19" s="50"/>
+      <c r="A19" s="48"/>
+      <c r="B19" s="48"/>
+      <c r="C19" s="48"/>
+      <c r="D19" s="51"/>
+      <c r="E19" s="51"/>
+      <c r="F19" s="51"/>
+      <c r="G19" s="48"/>
+      <c r="H19" s="48"/>
+      <c r="I19" s="48"/>
+      <c r="J19" s="58"/>
+      <c r="K19" s="58"/>
+      <c r="L19" s="58"/>
+      <c r="M19" s="48"/>
+      <c r="N19" s="48"/>
+      <c r="O19" s="57"/>
+      <c r="P19" s="59"/>
+      <c r="Q19" s="60"/>
       <c r="R19" s="3"/>
       <c r="S19" s="3"/>
       <c r="T19" s="3"/>
@@ -30154,39 +30154,39 @@
       <c r="Z19" s="3"/>
     </row>
     <row r="20" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="58" t="s">
+      <c r="A20" s="47" t="s">
         <v>22</v>
       </c>
-      <c r="B20" s="55" t="s">
+      <c r="B20" s="49" t="s">
         <v>23</v>
       </c>
-      <c r="C20" s="51"/>
-      <c r="D20" s="56" t="s">
+      <c r="C20" s="48"/>
+      <c r="D20" s="50" t="s">
         <v>63</v>
       </c>
-      <c r="E20" s="57"/>
-      <c r="F20" s="57"/>
-      <c r="G20" s="54" t="s">
+      <c r="E20" s="51"/>
+      <c r="F20" s="51"/>
+      <c r="G20" s="53" t="s">
         <v>24</v>
       </c>
-      <c r="H20" s="51"/>
-      <c r="I20" s="51"/>
-      <c r="J20" s="53" t="s">
+      <c r="H20" s="48"/>
+      <c r="I20" s="48"/>
+      <c r="J20" s="52" t="s">
         <v>25</v>
       </c>
-      <c r="K20" s="51"/>
-      <c r="L20" s="51"/>
-      <c r="M20" s="54" t="s">
+      <c r="K20" s="48"/>
+      <c r="L20" s="48"/>
+      <c r="M20" s="53" t="s">
         <v>26</v>
       </c>
-      <c r="N20" s="51"/>
-      <c r="O20" s="47" t="s">
+      <c r="N20" s="48"/>
+      <c r="O20" s="56" t="s">
         <v>26</v>
       </c>
-      <c r="P20" s="49" t="s">
+      <c r="P20" s="59" t="s">
         <v>66</v>
       </c>
-      <c r="Q20" s="50"/>
+      <c r="Q20" s="60"/>
       <c r="R20" s="3"/>
       <c r="S20" s="3"/>
       <c r="T20" s="3"/>
@@ -30198,23 +30198,23 @@
       <c r="Z20" s="3"/>
     </row>
     <row r="21" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="51"/>
-      <c r="B21" s="51"/>
-      <c r="C21" s="51"/>
-      <c r="D21" s="57"/>
-      <c r="E21" s="57"/>
-      <c r="F21" s="57"/>
-      <c r="G21" s="51"/>
-      <c r="H21" s="51"/>
-      <c r="I21" s="51"/>
-      <c r="J21" s="51"/>
-      <c r="K21" s="51"/>
-      <c r="L21" s="51"/>
-      <c r="M21" s="51"/>
-      <c r="N21" s="51"/>
-      <c r="O21" s="48"/>
-      <c r="P21" s="49"/>
-      <c r="Q21" s="50"/>
+      <c r="A21" s="48"/>
+      <c r="B21" s="48"/>
+      <c r="C21" s="48"/>
+      <c r="D21" s="51"/>
+      <c r="E21" s="51"/>
+      <c r="F21" s="51"/>
+      <c r="G21" s="48"/>
+      <c r="H21" s="48"/>
+      <c r="I21" s="48"/>
+      <c r="J21" s="48"/>
+      <c r="K21" s="48"/>
+      <c r="L21" s="48"/>
+      <c r="M21" s="48"/>
+      <c r="N21" s="48"/>
+      <c r="O21" s="57"/>
+      <c r="P21" s="59"/>
+      <c r="Q21" s="60"/>
       <c r="R21" s="3"/>
       <c r="S21" s="3"/>
       <c r="T21" s="3"/>
@@ -30226,23 +30226,23 @@
       <c r="Z21" s="3"/>
     </row>
     <row r="22" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="51"/>
-      <c r="B22" s="51"/>
-      <c r="C22" s="51"/>
-      <c r="D22" s="57"/>
-      <c r="E22" s="57"/>
-      <c r="F22" s="57"/>
-      <c r="G22" s="51"/>
-      <c r="H22" s="51"/>
-      <c r="I22" s="51"/>
-      <c r="J22" s="51"/>
-      <c r="K22" s="51"/>
-      <c r="L22" s="51"/>
-      <c r="M22" s="51"/>
-      <c r="N22" s="51"/>
-      <c r="O22" s="48"/>
-      <c r="P22" s="49"/>
-      <c r="Q22" s="50"/>
+      <c r="A22" s="48"/>
+      <c r="B22" s="48"/>
+      <c r="C22" s="48"/>
+      <c r="D22" s="51"/>
+      <c r="E22" s="51"/>
+      <c r="F22" s="51"/>
+      <c r="G22" s="48"/>
+      <c r="H22" s="48"/>
+      <c r="I22" s="48"/>
+      <c r="J22" s="48"/>
+      <c r="K22" s="48"/>
+      <c r="L22" s="48"/>
+      <c r="M22" s="48"/>
+      <c r="N22" s="48"/>
+      <c r="O22" s="57"/>
+      <c r="P22" s="59"/>
+      <c r="Q22" s="60"/>
       <c r="R22" s="3"/>
       <c r="S22" s="3"/>
       <c r="T22" s="3"/>
@@ -30254,23 +30254,23 @@
       <c r="Z22" s="3"/>
     </row>
     <row r="23" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="51"/>
-      <c r="B23" s="51"/>
-      <c r="C23" s="51"/>
-      <c r="D23" s="57"/>
-      <c r="E23" s="57"/>
-      <c r="F23" s="57"/>
-      <c r="G23" s="51"/>
-      <c r="H23" s="51"/>
-      <c r="I23" s="51"/>
-      <c r="J23" s="51"/>
-      <c r="K23" s="51"/>
-      <c r="L23" s="51"/>
-      <c r="M23" s="51"/>
-      <c r="N23" s="51"/>
-      <c r="O23" s="48"/>
-      <c r="P23" s="49"/>
-      <c r="Q23" s="50"/>
+      <c r="A23" s="48"/>
+      <c r="B23" s="48"/>
+      <c r="C23" s="48"/>
+      <c r="D23" s="51"/>
+      <c r="E23" s="51"/>
+      <c r="F23" s="51"/>
+      <c r="G23" s="48"/>
+      <c r="H23" s="48"/>
+      <c r="I23" s="48"/>
+      <c r="J23" s="48"/>
+      <c r="K23" s="48"/>
+      <c r="L23" s="48"/>
+      <c r="M23" s="48"/>
+      <c r="N23" s="48"/>
+      <c r="O23" s="57"/>
+      <c r="P23" s="59"/>
+      <c r="Q23" s="60"/>
       <c r="R23" s="3"/>
       <c r="S23" s="3"/>
       <c r="T23" s="3"/>
@@ -30282,23 +30282,23 @@
       <c r="Z23" s="3"/>
     </row>
     <row r="24" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="51"/>
-      <c r="B24" s="51"/>
-      <c r="C24" s="51"/>
-      <c r="D24" s="57"/>
-      <c r="E24" s="57"/>
-      <c r="F24" s="57"/>
-      <c r="G24" s="51"/>
-      <c r="H24" s="51"/>
-      <c r="I24" s="51"/>
-      <c r="J24" s="51"/>
-      <c r="K24" s="51"/>
-      <c r="L24" s="51"/>
-      <c r="M24" s="51"/>
-      <c r="N24" s="51"/>
-      <c r="O24" s="48"/>
-      <c r="P24" s="49"/>
-      <c r="Q24" s="50"/>
+      <c r="A24" s="48"/>
+      <c r="B24" s="48"/>
+      <c r="C24" s="48"/>
+      <c r="D24" s="51"/>
+      <c r="E24" s="51"/>
+      <c r="F24" s="51"/>
+      <c r="G24" s="48"/>
+      <c r="H24" s="48"/>
+      <c r="I24" s="48"/>
+      <c r="J24" s="48"/>
+      <c r="K24" s="48"/>
+      <c r="L24" s="48"/>
+      <c r="M24" s="48"/>
+      <c r="N24" s="48"/>
+      <c r="O24" s="57"/>
+      <c r="P24" s="59"/>
+      <c r="Q24" s="60"/>
       <c r="R24" s="3"/>
       <c r="S24" s="3"/>
       <c r="T24" s="3"/>
@@ -30310,23 +30310,23 @@
       <c r="Z24" s="3"/>
     </row>
     <row r="25" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="51"/>
-      <c r="B25" s="51"/>
-      <c r="C25" s="51"/>
-      <c r="D25" s="57"/>
-      <c r="E25" s="57"/>
-      <c r="F25" s="57"/>
-      <c r="G25" s="51"/>
-      <c r="H25" s="51"/>
-      <c r="I25" s="51"/>
-      <c r="J25" s="51"/>
-      <c r="K25" s="51"/>
-      <c r="L25" s="51"/>
-      <c r="M25" s="51"/>
-      <c r="N25" s="51"/>
-      <c r="O25" s="48"/>
-      <c r="P25" s="49"/>
-      <c r="Q25" s="50"/>
+      <c r="A25" s="48"/>
+      <c r="B25" s="48"/>
+      <c r="C25" s="48"/>
+      <c r="D25" s="51"/>
+      <c r="E25" s="51"/>
+      <c r="F25" s="51"/>
+      <c r="G25" s="48"/>
+      <c r="H25" s="48"/>
+      <c r="I25" s="48"/>
+      <c r="J25" s="48"/>
+      <c r="K25" s="48"/>
+      <c r="L25" s="48"/>
+      <c r="M25" s="48"/>
+      <c r="N25" s="48"/>
+      <c r="O25" s="57"/>
+      <c r="P25" s="59"/>
+      <c r="Q25" s="60"/>
       <c r="R25" s="3"/>
       <c r="S25" s="3"/>
       <c r="T25" s="3"/>
@@ -30338,39 +30338,39 @@
       <c r="Z25" s="3"/>
     </row>
     <row r="26" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="58" t="s">
+      <c r="A26" s="47" t="s">
         <v>27</v>
       </c>
-      <c r="B26" s="53" t="s">
+      <c r="B26" s="52" t="s">
         <v>28</v>
       </c>
-      <c r="C26" s="51"/>
-      <c r="D26" s="56" t="s">
+      <c r="C26" s="48"/>
+      <c r="D26" s="50" t="s">
         <v>63</v>
       </c>
-      <c r="E26" s="57"/>
-      <c r="F26" s="57"/>
-      <c r="G26" s="53" t="s">
+      <c r="E26" s="51"/>
+      <c r="F26" s="51"/>
+      <c r="G26" s="52" t="s">
         <v>29</v>
       </c>
-      <c r="H26" s="51"/>
-      <c r="I26" s="51"/>
-      <c r="J26" s="49" t="s">
+      <c r="H26" s="48"/>
+      <c r="I26" s="48"/>
+      <c r="J26" s="59" t="s">
         <v>20</v>
       </c>
-      <c r="K26" s="51"/>
-      <c r="L26" s="51"/>
-      <c r="M26" s="54" t="s">
+      <c r="K26" s="48"/>
+      <c r="L26" s="48"/>
+      <c r="M26" s="53" t="s">
         <v>30</v>
       </c>
-      <c r="N26" s="51"/>
-      <c r="O26" s="47" t="s">
+      <c r="N26" s="48"/>
+      <c r="O26" s="56" t="s">
         <v>30</v>
       </c>
-      <c r="P26" s="49" t="s">
+      <c r="P26" s="59" t="s">
         <v>66</v>
       </c>
-      <c r="Q26" s="50"/>
+      <c r="Q26" s="60"/>
       <c r="R26" s="3"/>
       <c r="S26" s="3"/>
       <c r="T26" s="3"/>
@@ -30382,23 +30382,23 @@
       <c r="Z26" s="3"/>
     </row>
     <row r="27" spans="1:26" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A27" s="51"/>
-      <c r="B27" s="51"/>
-      <c r="C27" s="51"/>
-      <c r="D27" s="57"/>
-      <c r="E27" s="57"/>
-      <c r="F27" s="57"/>
-      <c r="G27" s="51"/>
-      <c r="H27" s="51"/>
-      <c r="I27" s="51"/>
-      <c r="J27" s="51"/>
-      <c r="K27" s="51"/>
-      <c r="L27" s="51"/>
-      <c r="M27" s="51"/>
-      <c r="N27" s="51"/>
-      <c r="O27" s="48"/>
-      <c r="P27" s="49"/>
-      <c r="Q27" s="50"/>
+      <c r="A27" s="48"/>
+      <c r="B27" s="48"/>
+      <c r="C27" s="48"/>
+      <c r="D27" s="51"/>
+      <c r="E27" s="51"/>
+      <c r="F27" s="51"/>
+      <c r="G27" s="48"/>
+      <c r="H27" s="48"/>
+      <c r="I27" s="48"/>
+      <c r="J27" s="48"/>
+      <c r="K27" s="48"/>
+      <c r="L27" s="48"/>
+      <c r="M27" s="48"/>
+      <c r="N27" s="48"/>
+      <c r="O27" s="57"/>
+      <c r="P27" s="59"/>
+      <c r="Q27" s="60"/>
       <c r="R27" s="3"/>
       <c r="S27" s="3"/>
       <c r="T27" s="3"/>
@@ -30410,23 +30410,23 @@
       <c r="Z27" s="3"/>
     </row>
     <row r="28" spans="1:26" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A28" s="51"/>
-      <c r="B28" s="51"/>
-      <c r="C28" s="51"/>
-      <c r="D28" s="57"/>
-      <c r="E28" s="57"/>
-      <c r="F28" s="57"/>
-      <c r="G28" s="51"/>
-      <c r="H28" s="51"/>
-      <c r="I28" s="51"/>
-      <c r="J28" s="51"/>
-      <c r="K28" s="51"/>
-      <c r="L28" s="51"/>
-      <c r="M28" s="51"/>
-      <c r="N28" s="51"/>
-      <c r="O28" s="48"/>
-      <c r="P28" s="49"/>
-      <c r="Q28" s="50"/>
+      <c r="A28" s="48"/>
+      <c r="B28" s="48"/>
+      <c r="C28" s="48"/>
+      <c r="D28" s="51"/>
+      <c r="E28" s="51"/>
+      <c r="F28" s="51"/>
+      <c r="G28" s="48"/>
+      <c r="H28" s="48"/>
+      <c r="I28" s="48"/>
+      <c r="J28" s="48"/>
+      <c r="K28" s="48"/>
+      <c r="L28" s="48"/>
+      <c r="M28" s="48"/>
+      <c r="N28" s="48"/>
+      <c r="O28" s="57"/>
+      <c r="P28" s="59"/>
+      <c r="Q28" s="60"/>
       <c r="R28" s="3"/>
       <c r="S28" s="3"/>
       <c r="T28" s="3"/>
@@ -30438,23 +30438,23 @@
       <c r="Z28" s="3"/>
     </row>
     <row r="29" spans="1:26" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A29" s="51"/>
-      <c r="B29" s="51"/>
-      <c r="C29" s="51"/>
-      <c r="D29" s="57"/>
-      <c r="E29" s="57"/>
-      <c r="F29" s="57"/>
-      <c r="G29" s="51"/>
-      <c r="H29" s="51"/>
-      <c r="I29" s="51"/>
-      <c r="J29" s="51"/>
-      <c r="K29" s="51"/>
-      <c r="L29" s="51"/>
-      <c r="M29" s="51"/>
-      <c r="N29" s="51"/>
-      <c r="O29" s="48"/>
-      <c r="P29" s="49"/>
-      <c r="Q29" s="50"/>
+      <c r="A29" s="48"/>
+      <c r="B29" s="48"/>
+      <c r="C29" s="48"/>
+      <c r="D29" s="51"/>
+      <c r="E29" s="51"/>
+      <c r="F29" s="51"/>
+      <c r="G29" s="48"/>
+      <c r="H29" s="48"/>
+      <c r="I29" s="48"/>
+      <c r="J29" s="48"/>
+      <c r="K29" s="48"/>
+      <c r="L29" s="48"/>
+      <c r="M29" s="48"/>
+      <c r="N29" s="48"/>
+      <c r="O29" s="57"/>
+      <c r="P29" s="59"/>
+      <c r="Q29" s="60"/>
       <c r="R29" s="3"/>
       <c r="S29" s="3"/>
       <c r="T29" s="3"/>
@@ -30466,23 +30466,23 @@
       <c r="Z29" s="3"/>
     </row>
     <row r="30" spans="1:26" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A30" s="51"/>
-      <c r="B30" s="51"/>
-      <c r="C30" s="51"/>
-      <c r="D30" s="57"/>
-      <c r="E30" s="57"/>
-      <c r="F30" s="57"/>
-      <c r="G30" s="51"/>
-      <c r="H30" s="51"/>
-      <c r="I30" s="51"/>
-      <c r="J30" s="51"/>
-      <c r="K30" s="51"/>
-      <c r="L30" s="51"/>
-      <c r="M30" s="51"/>
-      <c r="N30" s="51"/>
-      <c r="O30" s="48"/>
-      <c r="P30" s="49"/>
-      <c r="Q30" s="50"/>
+      <c r="A30" s="48"/>
+      <c r="B30" s="48"/>
+      <c r="C30" s="48"/>
+      <c r="D30" s="51"/>
+      <c r="E30" s="51"/>
+      <c r="F30" s="51"/>
+      <c r="G30" s="48"/>
+      <c r="H30" s="48"/>
+      <c r="I30" s="48"/>
+      <c r="J30" s="48"/>
+      <c r="K30" s="48"/>
+      <c r="L30" s="48"/>
+      <c r="M30" s="48"/>
+      <c r="N30" s="48"/>
+      <c r="O30" s="57"/>
+      <c r="P30" s="59"/>
+      <c r="Q30" s="60"/>
       <c r="R30" s="3"/>
       <c r="S30" s="3"/>
       <c r="T30" s="3"/>
@@ -30494,23 +30494,23 @@
       <c r="Z30" s="3"/>
     </row>
     <row r="31" spans="1:26" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A31" s="51"/>
-      <c r="B31" s="51"/>
-      <c r="C31" s="51"/>
-      <c r="D31" s="57"/>
-      <c r="E31" s="57"/>
-      <c r="F31" s="57"/>
-      <c r="G31" s="51"/>
-      <c r="H31" s="51"/>
-      <c r="I31" s="51"/>
-      <c r="J31" s="51"/>
-      <c r="K31" s="51"/>
-      <c r="L31" s="51"/>
-      <c r="M31" s="51"/>
-      <c r="N31" s="51"/>
-      <c r="O31" s="48"/>
-      <c r="P31" s="49"/>
-      <c r="Q31" s="50"/>
+      <c r="A31" s="48"/>
+      <c r="B31" s="48"/>
+      <c r="C31" s="48"/>
+      <c r="D31" s="51"/>
+      <c r="E31" s="51"/>
+      <c r="F31" s="51"/>
+      <c r="G31" s="48"/>
+      <c r="H31" s="48"/>
+      <c r="I31" s="48"/>
+      <c r="J31" s="48"/>
+      <c r="K31" s="48"/>
+      <c r="L31" s="48"/>
+      <c r="M31" s="48"/>
+      <c r="N31" s="48"/>
+      <c r="O31" s="57"/>
+      <c r="P31" s="59"/>
+      <c r="Q31" s="60"/>
       <c r="R31" s="3"/>
       <c r="S31" s="3"/>
       <c r="T31" s="3"/>
@@ -30522,39 +30522,39 @@
       <c r="Z31" s="3"/>
     </row>
     <row r="32" spans="1:26" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="58" t="s">
+      <c r="A32" s="47" t="s">
         <v>31</v>
       </c>
-      <c r="B32" s="55" t="s">
+      <c r="B32" s="49" t="s">
         <v>32</v>
       </c>
-      <c r="C32" s="51"/>
-      <c r="D32" s="56" t="s">
+      <c r="C32" s="48"/>
+      <c r="D32" s="50" t="s">
         <v>63</v>
       </c>
-      <c r="E32" s="57"/>
-      <c r="F32" s="57"/>
-      <c r="G32" s="53" t="s">
+      <c r="E32" s="51"/>
+      <c r="F32" s="51"/>
+      <c r="G32" s="52" t="s">
         <v>33</v>
       </c>
-      <c r="H32" s="51"/>
-      <c r="I32" s="51"/>
-      <c r="J32" s="53" t="s">
+      <c r="H32" s="48"/>
+      <c r="I32" s="48"/>
+      <c r="J32" s="52" t="s">
         <v>34</v>
       </c>
-      <c r="K32" s="51"/>
-      <c r="L32" s="51"/>
-      <c r="M32" s="54" t="s">
+      <c r="K32" s="48"/>
+      <c r="L32" s="48"/>
+      <c r="M32" s="53" t="s">
         <v>65</v>
       </c>
-      <c r="N32" s="51"/>
-      <c r="O32" s="47" t="s">
+      <c r="N32" s="48"/>
+      <c r="O32" s="56" t="s">
         <v>65</v>
       </c>
-      <c r="P32" s="49" t="s">
+      <c r="P32" s="59" t="s">
         <v>66</v>
       </c>
-      <c r="Q32" s="50"/>
+      <c r="Q32" s="60"/>
       <c r="R32" s="3"/>
       <c r="S32" s="3"/>
       <c r="T32" s="3"/>
@@ -30566,23 +30566,23 @@
       <c r="Z32" s="3"/>
     </row>
     <row r="33" spans="1:26" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A33" s="51"/>
-      <c r="B33" s="51"/>
-      <c r="C33" s="51"/>
-      <c r="D33" s="57"/>
-      <c r="E33" s="57"/>
-      <c r="F33" s="57"/>
-      <c r="G33" s="51"/>
-      <c r="H33" s="51"/>
-      <c r="I33" s="51"/>
-      <c r="J33" s="51"/>
-      <c r="K33" s="51"/>
-      <c r="L33" s="51"/>
-      <c r="M33" s="51"/>
-      <c r="N33" s="51"/>
-      <c r="O33" s="48"/>
-      <c r="P33" s="49"/>
-      <c r="Q33" s="50"/>
+      <c r="A33" s="48"/>
+      <c r="B33" s="48"/>
+      <c r="C33" s="48"/>
+      <c r="D33" s="51"/>
+      <c r="E33" s="51"/>
+      <c r="F33" s="51"/>
+      <c r="G33" s="48"/>
+      <c r="H33" s="48"/>
+      <c r="I33" s="48"/>
+      <c r="J33" s="48"/>
+      <c r="K33" s="48"/>
+      <c r="L33" s="48"/>
+      <c r="M33" s="48"/>
+      <c r="N33" s="48"/>
+      <c r="O33" s="57"/>
+      <c r="P33" s="59"/>
+      <c r="Q33" s="60"/>
       <c r="R33" s="3"/>
       <c r="S33" s="3"/>
       <c r="T33" s="3"/>
@@ -30594,23 +30594,23 @@
       <c r="Z33" s="3"/>
     </row>
     <row r="34" spans="1:26" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A34" s="51"/>
-      <c r="B34" s="51"/>
-      <c r="C34" s="51"/>
-      <c r="D34" s="57"/>
-      <c r="E34" s="57"/>
-      <c r="F34" s="57"/>
-      <c r="G34" s="51"/>
-      <c r="H34" s="51"/>
-      <c r="I34" s="51"/>
-      <c r="J34" s="51"/>
-      <c r="K34" s="51"/>
-      <c r="L34" s="51"/>
-      <c r="M34" s="51"/>
-      <c r="N34" s="51"/>
-      <c r="O34" s="48"/>
-      <c r="P34" s="49"/>
-      <c r="Q34" s="50"/>
+      <c r="A34" s="48"/>
+      <c r="B34" s="48"/>
+      <c r="C34" s="48"/>
+      <c r="D34" s="51"/>
+      <c r="E34" s="51"/>
+      <c r="F34" s="51"/>
+      <c r="G34" s="48"/>
+      <c r="H34" s="48"/>
+      <c r="I34" s="48"/>
+      <c r="J34" s="48"/>
+      <c r="K34" s="48"/>
+      <c r="L34" s="48"/>
+      <c r="M34" s="48"/>
+      <c r="N34" s="48"/>
+      <c r="O34" s="57"/>
+      <c r="P34" s="59"/>
+      <c r="Q34" s="60"/>
       <c r="R34" s="3"/>
       <c r="S34" s="3"/>
       <c r="T34" s="3"/>
@@ -30622,23 +30622,23 @@
       <c r="Z34" s="3"/>
     </row>
     <row r="35" spans="1:26" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A35" s="51"/>
-      <c r="B35" s="51"/>
-      <c r="C35" s="51"/>
-      <c r="D35" s="57"/>
-      <c r="E35" s="57"/>
-      <c r="F35" s="57"/>
-      <c r="G35" s="51"/>
-      <c r="H35" s="51"/>
-      <c r="I35" s="51"/>
-      <c r="J35" s="51"/>
-      <c r="K35" s="51"/>
-      <c r="L35" s="51"/>
-      <c r="M35" s="51"/>
-      <c r="N35" s="51"/>
-      <c r="O35" s="48"/>
-      <c r="P35" s="49"/>
-      <c r="Q35" s="50"/>
+      <c r="A35" s="48"/>
+      <c r="B35" s="48"/>
+      <c r="C35" s="48"/>
+      <c r="D35" s="51"/>
+      <c r="E35" s="51"/>
+      <c r="F35" s="51"/>
+      <c r="G35" s="48"/>
+      <c r="H35" s="48"/>
+      <c r="I35" s="48"/>
+      <c r="J35" s="48"/>
+      <c r="K35" s="48"/>
+      <c r="L35" s="48"/>
+      <c r="M35" s="48"/>
+      <c r="N35" s="48"/>
+      <c r="O35" s="57"/>
+      <c r="P35" s="59"/>
+      <c r="Q35" s="60"/>
       <c r="R35" s="3"/>
       <c r="S35" s="3"/>
       <c r="T35" s="3"/>
@@ -30650,23 +30650,23 @@
       <c r="Z35" s="3"/>
     </row>
     <row r="36" spans="1:26" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A36" s="51"/>
-      <c r="B36" s="51"/>
-      <c r="C36" s="51"/>
-      <c r="D36" s="57"/>
-      <c r="E36" s="57"/>
-      <c r="F36" s="57"/>
-      <c r="G36" s="51"/>
-      <c r="H36" s="51"/>
-      <c r="I36" s="51"/>
-      <c r="J36" s="51"/>
-      <c r="K36" s="51"/>
-      <c r="L36" s="51"/>
-      <c r="M36" s="51"/>
-      <c r="N36" s="51"/>
-      <c r="O36" s="48"/>
-      <c r="P36" s="49"/>
-      <c r="Q36" s="50"/>
+      <c r="A36" s="48"/>
+      <c r="B36" s="48"/>
+      <c r="C36" s="48"/>
+      <c r="D36" s="51"/>
+      <c r="E36" s="51"/>
+      <c r="F36" s="51"/>
+      <c r="G36" s="48"/>
+      <c r="H36" s="48"/>
+      <c r="I36" s="48"/>
+      <c r="J36" s="48"/>
+      <c r="K36" s="48"/>
+      <c r="L36" s="48"/>
+      <c r="M36" s="48"/>
+      <c r="N36" s="48"/>
+      <c r="O36" s="57"/>
+      <c r="P36" s="59"/>
+      <c r="Q36" s="60"/>
       <c r="R36" s="3"/>
       <c r="S36" s="3"/>
       <c r="T36" s="3"/>
@@ -30678,23 +30678,23 @@
       <c r="Z36" s="3"/>
     </row>
     <row r="37" spans="1:26" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A37" s="51"/>
-      <c r="B37" s="51"/>
-      <c r="C37" s="51"/>
-      <c r="D37" s="57"/>
-      <c r="E37" s="57"/>
-      <c r="F37" s="57"/>
-      <c r="G37" s="51"/>
-      <c r="H37" s="51"/>
-      <c r="I37" s="51"/>
-      <c r="J37" s="51"/>
-      <c r="K37" s="51"/>
-      <c r="L37" s="51"/>
-      <c r="M37" s="51"/>
-      <c r="N37" s="51"/>
-      <c r="O37" s="48"/>
-      <c r="P37" s="49"/>
-      <c r="Q37" s="50"/>
+      <c r="A37" s="48"/>
+      <c r="B37" s="48"/>
+      <c r="C37" s="48"/>
+      <c r="D37" s="51"/>
+      <c r="E37" s="51"/>
+      <c r="F37" s="51"/>
+      <c r="G37" s="48"/>
+      <c r="H37" s="48"/>
+      <c r="I37" s="48"/>
+      <c r="J37" s="48"/>
+      <c r="K37" s="48"/>
+      <c r="L37" s="48"/>
+      <c r="M37" s="48"/>
+      <c r="N37" s="48"/>
+      <c r="O37" s="57"/>
+      <c r="P37" s="59"/>
+      <c r="Q37" s="60"/>
       <c r="R37" s="3"/>
       <c r="S37" s="3"/>
       <c r="T37" s="3"/>
@@ -30706,39 +30706,39 @@
       <c r="Z37" s="3"/>
     </row>
     <row r="38" spans="1:26" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="58" t="s">
+      <c r="A38" s="47" t="s">
         <v>35</v>
       </c>
-      <c r="B38" s="53" t="s">
+      <c r="B38" s="52" t="s">
         <v>36</v>
       </c>
-      <c r="C38" s="51"/>
-      <c r="D38" s="56" t="s">
+      <c r="C38" s="48"/>
+      <c r="D38" s="50" t="s">
         <v>63</v>
       </c>
-      <c r="E38" s="57"/>
-      <c r="F38" s="57"/>
-      <c r="G38" s="53" t="s">
+      <c r="E38" s="51"/>
+      <c r="F38" s="51"/>
+      <c r="G38" s="52" t="s">
         <v>37</v>
       </c>
-      <c r="H38" s="51"/>
-      <c r="I38" s="51"/>
-      <c r="J38" s="53" t="s">
+      <c r="H38" s="48"/>
+      <c r="I38" s="48"/>
+      <c r="J38" s="52" t="s">
         <v>38</v>
       </c>
-      <c r="K38" s="51"/>
-      <c r="L38" s="51"/>
-      <c r="M38" s="54" t="s">
+      <c r="K38" s="48"/>
+      <c r="L38" s="48"/>
+      <c r="M38" s="53" t="s">
         <v>39</v>
       </c>
-      <c r="N38" s="51"/>
-      <c r="O38" s="47" t="s">
+      <c r="N38" s="48"/>
+      <c r="O38" s="56" t="s">
         <v>39</v>
       </c>
-      <c r="P38" s="49" t="s">
+      <c r="P38" s="59" t="s">
         <v>66</v>
       </c>
-      <c r="Q38" s="50"/>
+      <c r="Q38" s="60"/>
       <c r="R38" s="3"/>
       <c r="S38" s="3"/>
       <c r="T38" s="3"/>
@@ -30750,23 +30750,23 @@
       <c r="Z38" s="3"/>
     </row>
     <row r="39" spans="1:26" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A39" s="51"/>
-      <c r="B39" s="51"/>
-      <c r="C39" s="51"/>
-      <c r="D39" s="57"/>
-      <c r="E39" s="57"/>
-      <c r="F39" s="57"/>
-      <c r="G39" s="51"/>
-      <c r="H39" s="51"/>
-      <c r="I39" s="51"/>
-      <c r="J39" s="51"/>
-      <c r="K39" s="51"/>
-      <c r="L39" s="51"/>
-      <c r="M39" s="51"/>
-      <c r="N39" s="51"/>
-      <c r="O39" s="48"/>
-      <c r="P39" s="49"/>
-      <c r="Q39" s="50"/>
+      <c r="A39" s="48"/>
+      <c r="B39" s="48"/>
+      <c r="C39" s="48"/>
+      <c r="D39" s="51"/>
+      <c r="E39" s="51"/>
+      <c r="F39" s="51"/>
+      <c r="G39" s="48"/>
+      <c r="H39" s="48"/>
+      <c r="I39" s="48"/>
+      <c r="J39" s="48"/>
+      <c r="K39" s="48"/>
+      <c r="L39" s="48"/>
+      <c r="M39" s="48"/>
+      <c r="N39" s="48"/>
+      <c r="O39" s="57"/>
+      <c r="P39" s="59"/>
+      <c r="Q39" s="60"/>
       <c r="R39" s="3"/>
       <c r="S39" s="3"/>
       <c r="T39" s="3"/>
@@ -30778,23 +30778,23 @@
       <c r="Z39" s="3"/>
     </row>
     <row r="40" spans="1:26" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A40" s="51"/>
-      <c r="B40" s="51"/>
-      <c r="C40" s="51"/>
-      <c r="D40" s="57"/>
-      <c r="E40" s="57"/>
-      <c r="F40" s="57"/>
-      <c r="G40" s="51"/>
-      <c r="H40" s="51"/>
-      <c r="I40" s="51"/>
-      <c r="J40" s="51"/>
-      <c r="K40" s="51"/>
-      <c r="L40" s="51"/>
-      <c r="M40" s="51"/>
-      <c r="N40" s="51"/>
-      <c r="O40" s="48"/>
-      <c r="P40" s="49"/>
-      <c r="Q40" s="50"/>
+      <c r="A40" s="48"/>
+      <c r="B40" s="48"/>
+      <c r="C40" s="48"/>
+      <c r="D40" s="51"/>
+      <c r="E40" s="51"/>
+      <c r="F40" s="51"/>
+      <c r="G40" s="48"/>
+      <c r="H40" s="48"/>
+      <c r="I40" s="48"/>
+      <c r="J40" s="48"/>
+      <c r="K40" s="48"/>
+      <c r="L40" s="48"/>
+      <c r="M40" s="48"/>
+      <c r="N40" s="48"/>
+      <c r="O40" s="57"/>
+      <c r="P40" s="59"/>
+      <c r="Q40" s="60"/>
       <c r="R40" s="3"/>
       <c r="S40" s="3"/>
       <c r="T40" s="3"/>
@@ -30806,23 +30806,23 @@
       <c r="Z40" s="3"/>
     </row>
     <row r="41" spans="1:26" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A41" s="51"/>
-      <c r="B41" s="51"/>
-      <c r="C41" s="51"/>
-      <c r="D41" s="57"/>
-      <c r="E41" s="57"/>
-      <c r="F41" s="57"/>
-      <c r="G41" s="51"/>
-      <c r="H41" s="51"/>
-      <c r="I41" s="51"/>
-      <c r="J41" s="51"/>
-      <c r="K41" s="51"/>
-      <c r="L41" s="51"/>
-      <c r="M41" s="51"/>
-      <c r="N41" s="51"/>
-      <c r="O41" s="48"/>
-      <c r="P41" s="49"/>
-      <c r="Q41" s="50"/>
+      <c r="A41" s="48"/>
+      <c r="B41" s="48"/>
+      <c r="C41" s="48"/>
+      <c r="D41" s="51"/>
+      <c r="E41" s="51"/>
+      <c r="F41" s="51"/>
+      <c r="G41" s="48"/>
+      <c r="H41" s="48"/>
+      <c r="I41" s="48"/>
+      <c r="J41" s="48"/>
+      <c r="K41" s="48"/>
+      <c r="L41" s="48"/>
+      <c r="M41" s="48"/>
+      <c r="N41" s="48"/>
+      <c r="O41" s="57"/>
+      <c r="P41" s="59"/>
+      <c r="Q41" s="60"/>
       <c r="R41" s="3"/>
       <c r="S41" s="3"/>
       <c r="T41" s="3"/>
@@ -30834,23 +30834,23 @@
       <c r="Z41" s="3"/>
     </row>
     <row r="42" spans="1:26" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A42" s="51"/>
-      <c r="B42" s="51"/>
-      <c r="C42" s="51"/>
-      <c r="D42" s="57"/>
-      <c r="E42" s="57"/>
-      <c r="F42" s="57"/>
-      <c r="G42" s="51"/>
-      <c r="H42" s="51"/>
-      <c r="I42" s="51"/>
-      <c r="J42" s="51"/>
-      <c r="K42" s="51"/>
-      <c r="L42" s="51"/>
-      <c r="M42" s="51"/>
-      <c r="N42" s="51"/>
-      <c r="O42" s="48"/>
-      <c r="P42" s="49"/>
-      <c r="Q42" s="50"/>
+      <c r="A42" s="48"/>
+      <c r="B42" s="48"/>
+      <c r="C42" s="48"/>
+      <c r="D42" s="51"/>
+      <c r="E42" s="51"/>
+      <c r="F42" s="51"/>
+      <c r="G42" s="48"/>
+      <c r="H42" s="48"/>
+      <c r="I42" s="48"/>
+      <c r="J42" s="48"/>
+      <c r="K42" s="48"/>
+      <c r="L42" s="48"/>
+      <c r="M42" s="48"/>
+      <c r="N42" s="48"/>
+      <c r="O42" s="57"/>
+      <c r="P42" s="59"/>
+      <c r="Q42" s="60"/>
       <c r="R42" s="3"/>
       <c r="S42" s="3"/>
       <c r="T42" s="3"/>
@@ -30862,23 +30862,23 @@
       <c r="Z42" s="3"/>
     </row>
     <row r="43" spans="1:26" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A43" s="51"/>
-      <c r="B43" s="51"/>
-      <c r="C43" s="51"/>
-      <c r="D43" s="57"/>
-      <c r="E43" s="57"/>
-      <c r="F43" s="57"/>
-      <c r="G43" s="51"/>
-      <c r="H43" s="51"/>
-      <c r="I43" s="51"/>
-      <c r="J43" s="51"/>
-      <c r="K43" s="51"/>
-      <c r="L43" s="51"/>
-      <c r="M43" s="51"/>
-      <c r="N43" s="51"/>
-      <c r="O43" s="48"/>
-      <c r="P43" s="49"/>
-      <c r="Q43" s="50"/>
+      <c r="A43" s="48"/>
+      <c r="B43" s="48"/>
+      <c r="C43" s="48"/>
+      <c r="D43" s="51"/>
+      <c r="E43" s="51"/>
+      <c r="F43" s="51"/>
+      <c r="G43" s="48"/>
+      <c r="H43" s="48"/>
+      <c r="I43" s="48"/>
+      <c r="J43" s="48"/>
+      <c r="K43" s="48"/>
+      <c r="L43" s="48"/>
+      <c r="M43" s="48"/>
+      <c r="N43" s="48"/>
+      <c r="O43" s="57"/>
+      <c r="P43" s="59"/>
+      <c r="Q43" s="60"/>
       <c r="R43" s="3"/>
       <c r="S43" s="3"/>
       <c r="T43" s="3"/>
@@ -30890,39 +30890,39 @@
       <c r="Z43" s="3"/>
     </row>
     <row r="44" spans="1:26" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="58" t="s">
+      <c r="A44" s="47" t="s">
         <v>40</v>
       </c>
-      <c r="B44" s="55" t="s">
+      <c r="B44" s="49" t="s">
         <v>41</v>
       </c>
-      <c r="C44" s="51"/>
-      <c r="D44" s="56" t="s">
+      <c r="C44" s="48"/>
+      <c r="D44" s="50" t="s">
         <v>61</v>
       </c>
-      <c r="E44" s="57"/>
-      <c r="F44" s="57"/>
-      <c r="G44" s="54" t="s">
+      <c r="E44" s="51"/>
+      <c r="F44" s="51"/>
+      <c r="G44" s="53" t="s">
         <v>42</v>
       </c>
-      <c r="H44" s="51"/>
-      <c r="I44" s="51"/>
-      <c r="J44" s="53" t="s">
+      <c r="H44" s="48"/>
+      <c r="I44" s="48"/>
+      <c r="J44" s="52" t="s">
         <v>12</v>
       </c>
-      <c r="K44" s="51"/>
-      <c r="L44" s="51"/>
-      <c r="M44" s="54" t="s">
+      <c r="K44" s="48"/>
+      <c r="L44" s="48"/>
+      <c r="M44" s="53" t="s">
         <v>43</v>
       </c>
-      <c r="N44" s="51"/>
-      <c r="O44" s="47" t="s">
+      <c r="N44" s="48"/>
+      <c r="O44" s="56" t="s">
         <v>43</v>
       </c>
-      <c r="P44" s="49" t="s">
+      <c r="P44" s="59" t="s">
         <v>66</v>
       </c>
-      <c r="Q44" s="50"/>
+      <c r="Q44" s="60"/>
       <c r="R44" s="3"/>
       <c r="S44" s="3"/>
       <c r="T44" s="3"/>
@@ -30934,23 +30934,23 @@
       <c r="Z44" s="3"/>
     </row>
     <row r="45" spans="1:26" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A45" s="51"/>
-      <c r="B45" s="51"/>
-      <c r="C45" s="51"/>
-      <c r="D45" s="57"/>
-      <c r="E45" s="57"/>
-      <c r="F45" s="57"/>
-      <c r="G45" s="51"/>
-      <c r="H45" s="51"/>
-      <c r="I45" s="51"/>
-      <c r="J45" s="51"/>
-      <c r="K45" s="51"/>
-      <c r="L45" s="51"/>
-      <c r="M45" s="51"/>
-      <c r="N45" s="51"/>
-      <c r="O45" s="48"/>
-      <c r="P45" s="49"/>
-      <c r="Q45" s="50"/>
+      <c r="A45" s="48"/>
+      <c r="B45" s="48"/>
+      <c r="C45" s="48"/>
+      <c r="D45" s="51"/>
+      <c r="E45" s="51"/>
+      <c r="F45" s="51"/>
+      <c r="G45" s="48"/>
+      <c r="H45" s="48"/>
+      <c r="I45" s="48"/>
+      <c r="J45" s="48"/>
+      <c r="K45" s="48"/>
+      <c r="L45" s="48"/>
+      <c r="M45" s="48"/>
+      <c r="N45" s="48"/>
+      <c r="O45" s="57"/>
+      <c r="P45" s="59"/>
+      <c r="Q45" s="60"/>
       <c r="R45" s="3"/>
       <c r="S45" s="3"/>
       <c r="T45" s="3"/>
@@ -30962,23 +30962,23 @@
       <c r="Z45" s="3"/>
     </row>
     <row r="46" spans="1:26" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A46" s="51"/>
-      <c r="B46" s="51"/>
-      <c r="C46" s="51"/>
-      <c r="D46" s="57"/>
-      <c r="E46" s="57"/>
-      <c r="F46" s="57"/>
-      <c r="G46" s="51"/>
-      <c r="H46" s="51"/>
-      <c r="I46" s="51"/>
-      <c r="J46" s="51"/>
-      <c r="K46" s="51"/>
-      <c r="L46" s="51"/>
-      <c r="M46" s="51"/>
-      <c r="N46" s="51"/>
-      <c r="O46" s="48"/>
-      <c r="P46" s="49"/>
-      <c r="Q46" s="50"/>
+      <c r="A46" s="48"/>
+      <c r="B46" s="48"/>
+      <c r="C46" s="48"/>
+      <c r="D46" s="51"/>
+      <c r="E46" s="51"/>
+      <c r="F46" s="51"/>
+      <c r="G46" s="48"/>
+      <c r="H46" s="48"/>
+      <c r="I46" s="48"/>
+      <c r="J46" s="48"/>
+      <c r="K46" s="48"/>
+      <c r="L46" s="48"/>
+      <c r="M46" s="48"/>
+      <c r="N46" s="48"/>
+      <c r="O46" s="57"/>
+      <c r="P46" s="59"/>
+      <c r="Q46" s="60"/>
       <c r="R46" s="3"/>
       <c r="S46" s="3"/>
       <c r="T46" s="3"/>
@@ -30990,23 +30990,23 @@
       <c r="Z46" s="3"/>
     </row>
     <row r="47" spans="1:26" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A47" s="51"/>
-      <c r="B47" s="51"/>
-      <c r="C47" s="51"/>
-      <c r="D47" s="57"/>
-      <c r="E47" s="57"/>
-      <c r="F47" s="57"/>
-      <c r="G47" s="51"/>
-      <c r="H47" s="51"/>
-      <c r="I47" s="51"/>
-      <c r="J47" s="51"/>
-      <c r="K47" s="51"/>
-      <c r="L47" s="51"/>
-      <c r="M47" s="51"/>
-      <c r="N47" s="51"/>
-      <c r="O47" s="48"/>
-      <c r="P47" s="49"/>
-      <c r="Q47" s="50"/>
+      <c r="A47" s="48"/>
+      <c r="B47" s="48"/>
+      <c r="C47" s="48"/>
+      <c r="D47" s="51"/>
+      <c r="E47" s="51"/>
+      <c r="F47" s="51"/>
+      <c r="G47" s="48"/>
+      <c r="H47" s="48"/>
+      <c r="I47" s="48"/>
+      <c r="J47" s="48"/>
+      <c r="K47" s="48"/>
+      <c r="L47" s="48"/>
+      <c r="M47" s="48"/>
+      <c r="N47" s="48"/>
+      <c r="O47" s="57"/>
+      <c r="P47" s="59"/>
+      <c r="Q47" s="60"/>
       <c r="R47" s="3"/>
       <c r="S47" s="3"/>
       <c r="T47" s="3"/>
@@ -31018,23 +31018,23 @@
       <c r="Z47" s="3"/>
     </row>
     <row r="48" spans="1:26" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A48" s="51"/>
-      <c r="B48" s="51"/>
-      <c r="C48" s="51"/>
-      <c r="D48" s="57"/>
-      <c r="E48" s="57"/>
-      <c r="F48" s="57"/>
-      <c r="G48" s="51"/>
-      <c r="H48" s="51"/>
-      <c r="I48" s="51"/>
-      <c r="J48" s="51"/>
-      <c r="K48" s="51"/>
-      <c r="L48" s="51"/>
-      <c r="M48" s="51"/>
-      <c r="N48" s="51"/>
-      <c r="O48" s="48"/>
-      <c r="P48" s="49"/>
-      <c r="Q48" s="50"/>
+      <c r="A48" s="48"/>
+      <c r="B48" s="48"/>
+      <c r="C48" s="48"/>
+      <c r="D48" s="51"/>
+      <c r="E48" s="51"/>
+      <c r="F48" s="51"/>
+      <c r="G48" s="48"/>
+      <c r="H48" s="48"/>
+      <c r="I48" s="48"/>
+      <c r="J48" s="48"/>
+      <c r="K48" s="48"/>
+      <c r="L48" s="48"/>
+      <c r="M48" s="48"/>
+      <c r="N48" s="48"/>
+      <c r="O48" s="57"/>
+      <c r="P48" s="59"/>
+      <c r="Q48" s="60"/>
       <c r="R48" s="3"/>
       <c r="S48" s="3"/>
       <c r="T48" s="3"/>
@@ -31046,23 +31046,23 @@
       <c r="Z48" s="3"/>
     </row>
     <row r="49" spans="1:26" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A49" s="51"/>
-      <c r="B49" s="51"/>
-      <c r="C49" s="51"/>
-      <c r="D49" s="57"/>
-      <c r="E49" s="57"/>
-      <c r="F49" s="57"/>
-      <c r="G49" s="51"/>
-      <c r="H49" s="51"/>
-      <c r="I49" s="51"/>
-      <c r="J49" s="51"/>
-      <c r="K49" s="51"/>
-      <c r="L49" s="51"/>
-      <c r="M49" s="51"/>
-      <c r="N49" s="51"/>
-      <c r="O49" s="48"/>
-      <c r="P49" s="49"/>
-      <c r="Q49" s="50"/>
+      <c r="A49" s="48"/>
+      <c r="B49" s="48"/>
+      <c r="C49" s="48"/>
+      <c r="D49" s="51"/>
+      <c r="E49" s="51"/>
+      <c r="F49" s="51"/>
+      <c r="G49" s="48"/>
+      <c r="H49" s="48"/>
+      <c r="I49" s="48"/>
+      <c r="J49" s="48"/>
+      <c r="K49" s="48"/>
+      <c r="L49" s="48"/>
+      <c r="M49" s="48"/>
+      <c r="N49" s="48"/>
+      <c r="O49" s="57"/>
+      <c r="P49" s="59"/>
+      <c r="Q49" s="60"/>
       <c r="R49" s="3"/>
       <c r="S49" s="3"/>
       <c r="T49" s="3"/>
@@ -31074,39 +31074,39 @@
       <c r="Z49" s="3"/>
     </row>
     <row r="50" spans="1:26" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="58" t="s">
+      <c r="A50" s="47" t="s">
         <v>44</v>
       </c>
-      <c r="B50" s="55" t="s">
+      <c r="B50" s="49" t="s">
         <v>45</v>
       </c>
-      <c r="C50" s="51"/>
-      <c r="D50" s="56" t="s">
+      <c r="C50" s="48"/>
+      <c r="D50" s="50" t="s">
         <v>63</v>
       </c>
-      <c r="E50" s="57"/>
-      <c r="F50" s="57"/>
-      <c r="G50" s="53" t="s">
+      <c r="E50" s="51"/>
+      <c r="F50" s="51"/>
+      <c r="G50" s="52" t="s">
         <v>46</v>
       </c>
-      <c r="H50" s="51"/>
-      <c r="I50" s="51"/>
-      <c r="J50" s="53" t="s">
+      <c r="H50" s="48"/>
+      <c r="I50" s="48"/>
+      <c r="J50" s="52" t="s">
         <v>47</v>
       </c>
-      <c r="K50" s="51"/>
-      <c r="L50" s="51"/>
-      <c r="M50" s="54" t="s">
+      <c r="K50" s="48"/>
+      <c r="L50" s="48"/>
+      <c r="M50" s="53" t="s">
         <v>48</v>
       </c>
-      <c r="N50" s="51"/>
-      <c r="O50" s="47" t="s">
+      <c r="N50" s="48"/>
+      <c r="O50" s="56" t="s">
         <v>48</v>
       </c>
-      <c r="P50" s="49" t="s">
+      <c r="P50" s="59" t="s">
         <v>66</v>
       </c>
-      <c r="Q50" s="50"/>
+      <c r="Q50" s="60"/>
       <c r="R50" s="3"/>
       <c r="S50" s="3"/>
       <c r="T50" s="3"/>
@@ -31118,23 +31118,23 @@
       <c r="Z50" s="3"/>
     </row>
     <row r="51" spans="1:26" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A51" s="51"/>
-      <c r="B51" s="51"/>
-      <c r="C51" s="51"/>
-      <c r="D51" s="57"/>
-      <c r="E51" s="57"/>
-      <c r="F51" s="57"/>
-      <c r="G51" s="51"/>
-      <c r="H51" s="51"/>
-      <c r="I51" s="51"/>
-      <c r="J51" s="51"/>
-      <c r="K51" s="51"/>
-      <c r="L51" s="51"/>
-      <c r="M51" s="51"/>
-      <c r="N51" s="51"/>
-      <c r="O51" s="48"/>
-      <c r="P51" s="49"/>
-      <c r="Q51" s="50"/>
+      <c r="A51" s="48"/>
+      <c r="B51" s="48"/>
+      <c r="C51" s="48"/>
+      <c r="D51" s="51"/>
+      <c r="E51" s="51"/>
+      <c r="F51" s="51"/>
+      <c r="G51" s="48"/>
+      <c r="H51" s="48"/>
+      <c r="I51" s="48"/>
+      <c r="J51" s="48"/>
+      <c r="K51" s="48"/>
+      <c r="L51" s="48"/>
+      <c r="M51" s="48"/>
+      <c r="N51" s="48"/>
+      <c r="O51" s="57"/>
+      <c r="P51" s="59"/>
+      <c r="Q51" s="60"/>
       <c r="R51" s="3"/>
       <c r="S51" s="3"/>
       <c r="T51" s="3"/>
@@ -31146,23 +31146,23 @@
       <c r="Z51" s="3"/>
     </row>
     <row r="52" spans="1:26" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A52" s="51"/>
-      <c r="B52" s="51"/>
-      <c r="C52" s="51"/>
-      <c r="D52" s="57"/>
-      <c r="E52" s="57"/>
-      <c r="F52" s="57"/>
-      <c r="G52" s="51"/>
-      <c r="H52" s="51"/>
-      <c r="I52" s="51"/>
-      <c r="J52" s="51"/>
-      <c r="K52" s="51"/>
-      <c r="L52" s="51"/>
-      <c r="M52" s="51"/>
-      <c r="N52" s="51"/>
-      <c r="O52" s="48"/>
-      <c r="P52" s="49"/>
-      <c r="Q52" s="50"/>
+      <c r="A52" s="48"/>
+      <c r="B52" s="48"/>
+      <c r="C52" s="48"/>
+      <c r="D52" s="51"/>
+      <c r="E52" s="51"/>
+      <c r="F52" s="51"/>
+      <c r="G52" s="48"/>
+      <c r="H52" s="48"/>
+      <c r="I52" s="48"/>
+      <c r="J52" s="48"/>
+      <c r="K52" s="48"/>
+      <c r="L52" s="48"/>
+      <c r="M52" s="48"/>
+      <c r="N52" s="48"/>
+      <c r="O52" s="57"/>
+      <c r="P52" s="59"/>
+      <c r="Q52" s="60"/>
       <c r="R52" s="3"/>
       <c r="S52" s="3"/>
       <c r="T52" s="3"/>
@@ -31174,23 +31174,23 @@
       <c r="Z52" s="3"/>
     </row>
     <row r="53" spans="1:26" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A53" s="51"/>
-      <c r="B53" s="51"/>
-      <c r="C53" s="51"/>
-      <c r="D53" s="57"/>
-      <c r="E53" s="57"/>
-      <c r="F53" s="57"/>
-      <c r="G53" s="51"/>
-      <c r="H53" s="51"/>
-      <c r="I53" s="51"/>
-      <c r="J53" s="51"/>
-      <c r="K53" s="51"/>
-      <c r="L53" s="51"/>
-      <c r="M53" s="51"/>
-      <c r="N53" s="51"/>
-      <c r="O53" s="48"/>
-      <c r="P53" s="49"/>
-      <c r="Q53" s="50"/>
+      <c r="A53" s="48"/>
+      <c r="B53" s="48"/>
+      <c r="C53" s="48"/>
+      <c r="D53" s="51"/>
+      <c r="E53" s="51"/>
+      <c r="F53" s="51"/>
+      <c r="G53" s="48"/>
+      <c r="H53" s="48"/>
+      <c r="I53" s="48"/>
+      <c r="J53" s="48"/>
+      <c r="K53" s="48"/>
+      <c r="L53" s="48"/>
+      <c r="M53" s="48"/>
+      <c r="N53" s="48"/>
+      <c r="O53" s="57"/>
+      <c r="P53" s="59"/>
+      <c r="Q53" s="60"/>
       <c r="R53" s="3"/>
       <c r="S53" s="3"/>
       <c r="T53" s="3"/>
@@ -31202,23 +31202,23 @@
       <c r="Z53" s="3"/>
     </row>
     <row r="54" spans="1:26" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A54" s="51"/>
-      <c r="B54" s="51"/>
-      <c r="C54" s="51"/>
-      <c r="D54" s="57"/>
-      <c r="E54" s="57"/>
-      <c r="F54" s="57"/>
-      <c r="G54" s="51"/>
-      <c r="H54" s="51"/>
-      <c r="I54" s="51"/>
-      <c r="J54" s="51"/>
-      <c r="K54" s="51"/>
-      <c r="L54" s="51"/>
-      <c r="M54" s="51"/>
-      <c r="N54" s="51"/>
-      <c r="O54" s="48"/>
-      <c r="P54" s="49"/>
-      <c r="Q54" s="50"/>
+      <c r="A54" s="48"/>
+      <c r="B54" s="48"/>
+      <c r="C54" s="48"/>
+      <c r="D54" s="51"/>
+      <c r="E54" s="51"/>
+      <c r="F54" s="51"/>
+      <c r="G54" s="48"/>
+      <c r="H54" s="48"/>
+      <c r="I54" s="48"/>
+      <c r="J54" s="48"/>
+      <c r="K54" s="48"/>
+      <c r="L54" s="48"/>
+      <c r="M54" s="48"/>
+      <c r="N54" s="48"/>
+      <c r="O54" s="57"/>
+      <c r="P54" s="59"/>
+      <c r="Q54" s="60"/>
       <c r="R54" s="3"/>
       <c r="S54" s="3"/>
       <c r="T54" s="3"/>
@@ -31230,23 +31230,23 @@
       <c r="Z54" s="3"/>
     </row>
     <row r="55" spans="1:26" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A55" s="51"/>
-      <c r="B55" s="51"/>
-      <c r="C55" s="51"/>
-      <c r="D55" s="57"/>
-      <c r="E55" s="57"/>
-      <c r="F55" s="57"/>
-      <c r="G55" s="51"/>
-      <c r="H55" s="51"/>
-      <c r="I55" s="51"/>
-      <c r="J55" s="51"/>
-      <c r="K55" s="51"/>
-      <c r="L55" s="51"/>
-      <c r="M55" s="51"/>
-      <c r="N55" s="51"/>
-      <c r="O55" s="48"/>
-      <c r="P55" s="49"/>
-      <c r="Q55" s="50"/>
+      <c r="A55" s="48"/>
+      <c r="B55" s="48"/>
+      <c r="C55" s="48"/>
+      <c r="D55" s="51"/>
+      <c r="E55" s="51"/>
+      <c r="F55" s="51"/>
+      <c r="G55" s="48"/>
+      <c r="H55" s="48"/>
+      <c r="I55" s="48"/>
+      <c r="J55" s="48"/>
+      <c r="K55" s="48"/>
+      <c r="L55" s="48"/>
+      <c r="M55" s="48"/>
+      <c r="N55" s="48"/>
+      <c r="O55" s="57"/>
+      <c r="P55" s="59"/>
+      <c r="Q55" s="60"/>
       <c r="R55" s="3"/>
       <c r="S55" s="3"/>
       <c r="T55" s="3"/>
@@ -31258,39 +31258,39 @@
       <c r="Z55" s="3"/>
     </row>
     <row r="56" spans="1:26" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="58" t="s">
+      <c r="A56" s="47" t="s">
         <v>49</v>
       </c>
-      <c r="B56" s="53" t="s">
+      <c r="B56" s="52" t="s">
         <v>50</v>
       </c>
-      <c r="C56" s="51"/>
-      <c r="D56" s="56" t="s">
+      <c r="C56" s="48"/>
+      <c r="D56" s="50" t="s">
         <v>63</v>
       </c>
-      <c r="E56" s="57"/>
-      <c r="F56" s="57"/>
-      <c r="G56" s="53" t="s">
+      <c r="E56" s="51"/>
+      <c r="F56" s="51"/>
+      <c r="G56" s="52" t="s">
         <v>51</v>
       </c>
-      <c r="H56" s="51"/>
-      <c r="I56" s="51"/>
-      <c r="J56" s="53" t="s">
+      <c r="H56" s="48"/>
+      <c r="I56" s="48"/>
+      <c r="J56" s="52" t="s">
         <v>52</v>
       </c>
-      <c r="K56" s="51"/>
-      <c r="L56" s="51"/>
-      <c r="M56" s="54" t="s">
+      <c r="K56" s="48"/>
+      <c r="L56" s="48"/>
+      <c r="M56" s="53" t="s">
         <v>30</v>
       </c>
-      <c r="N56" s="51"/>
-      <c r="O56" s="47" t="s">
+      <c r="N56" s="48"/>
+      <c r="O56" s="56" t="s">
         <v>30</v>
       </c>
-      <c r="P56" s="49" t="s">
+      <c r="P56" s="59" t="s">
         <v>66</v>
       </c>
-      <c r="Q56" s="50"/>
+      <c r="Q56" s="60"/>
       <c r="R56" s="3"/>
       <c r="S56" s="3"/>
       <c r="T56" s="3"/>
@@ -31302,23 +31302,23 @@
       <c r="Z56" s="3"/>
     </row>
     <row r="57" spans="1:26" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A57" s="51"/>
-      <c r="B57" s="51"/>
-      <c r="C57" s="51"/>
-      <c r="D57" s="57"/>
-      <c r="E57" s="57"/>
-      <c r="F57" s="57"/>
-      <c r="G57" s="51"/>
-      <c r="H57" s="51"/>
-      <c r="I57" s="51"/>
-      <c r="J57" s="51"/>
-      <c r="K57" s="51"/>
-      <c r="L57" s="51"/>
-      <c r="M57" s="51"/>
-      <c r="N57" s="51"/>
-      <c r="O57" s="48"/>
-      <c r="P57" s="49"/>
-      <c r="Q57" s="50"/>
+      <c r="A57" s="48"/>
+      <c r="B57" s="48"/>
+      <c r="C57" s="48"/>
+      <c r="D57" s="51"/>
+      <c r="E57" s="51"/>
+      <c r="F57" s="51"/>
+      <c r="G57" s="48"/>
+      <c r="H57" s="48"/>
+      <c r="I57" s="48"/>
+      <c r="J57" s="48"/>
+      <c r="K57" s="48"/>
+      <c r="L57" s="48"/>
+      <c r="M57" s="48"/>
+      <c r="N57" s="48"/>
+      <c r="O57" s="57"/>
+      <c r="P57" s="59"/>
+      <c r="Q57" s="60"/>
       <c r="R57" s="3"/>
       <c r="S57" s="3"/>
       <c r="T57" s="3"/>
@@ -31330,23 +31330,23 @@
       <c r="Z57" s="3"/>
     </row>
     <row r="58" spans="1:26" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A58" s="51"/>
-      <c r="B58" s="51"/>
-      <c r="C58" s="51"/>
-      <c r="D58" s="57"/>
-      <c r="E58" s="57"/>
-      <c r="F58" s="57"/>
-      <c r="G58" s="51"/>
-      <c r="H58" s="51"/>
-      <c r="I58" s="51"/>
-      <c r="J58" s="51"/>
-      <c r="K58" s="51"/>
-      <c r="L58" s="51"/>
-      <c r="M58" s="51"/>
-      <c r="N58" s="51"/>
-      <c r="O58" s="48"/>
-      <c r="P58" s="49"/>
-      <c r="Q58" s="50"/>
+      <c r="A58" s="48"/>
+      <c r="B58" s="48"/>
+      <c r="C58" s="48"/>
+      <c r="D58" s="51"/>
+      <c r="E58" s="51"/>
+      <c r="F58" s="51"/>
+      <c r="G58" s="48"/>
+      <c r="H58" s="48"/>
+      <c r="I58" s="48"/>
+      <c r="J58" s="48"/>
+      <c r="K58" s="48"/>
+      <c r="L58" s="48"/>
+      <c r="M58" s="48"/>
+      <c r="N58" s="48"/>
+      <c r="O58" s="57"/>
+      <c r="P58" s="59"/>
+      <c r="Q58" s="60"/>
       <c r="R58" s="3"/>
       <c r="S58" s="3"/>
       <c r="T58" s="3"/>
@@ -31358,23 +31358,23 @@
       <c r="Z58" s="3"/>
     </row>
     <row r="59" spans="1:26" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A59" s="51"/>
-      <c r="B59" s="51"/>
-      <c r="C59" s="51"/>
-      <c r="D59" s="57"/>
-      <c r="E59" s="57"/>
-      <c r="F59" s="57"/>
-      <c r="G59" s="51"/>
-      <c r="H59" s="51"/>
-      <c r="I59" s="51"/>
-      <c r="J59" s="51"/>
-      <c r="K59" s="51"/>
-      <c r="L59" s="51"/>
-      <c r="M59" s="51"/>
-      <c r="N59" s="51"/>
-      <c r="O59" s="48"/>
-      <c r="P59" s="49"/>
-      <c r="Q59" s="50"/>
+      <c r="A59" s="48"/>
+      <c r="B59" s="48"/>
+      <c r="C59" s="48"/>
+      <c r="D59" s="51"/>
+      <c r="E59" s="51"/>
+      <c r="F59" s="51"/>
+      <c r="G59" s="48"/>
+      <c r="H59" s="48"/>
+      <c r="I59" s="48"/>
+      <c r="J59" s="48"/>
+      <c r="K59" s="48"/>
+      <c r="L59" s="48"/>
+      <c r="M59" s="48"/>
+      <c r="N59" s="48"/>
+      <c r="O59" s="57"/>
+      <c r="P59" s="59"/>
+      <c r="Q59" s="60"/>
       <c r="R59" s="3"/>
       <c r="S59" s="3"/>
       <c r="T59" s="3"/>
@@ -31386,23 +31386,23 @@
       <c r="Z59" s="3"/>
     </row>
     <row r="60" spans="1:26" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A60" s="51"/>
-      <c r="B60" s="51"/>
-      <c r="C60" s="51"/>
-      <c r="D60" s="57"/>
-      <c r="E60" s="57"/>
-      <c r="F60" s="57"/>
-      <c r="G60" s="51"/>
-      <c r="H60" s="51"/>
-      <c r="I60" s="51"/>
-      <c r="J60" s="51"/>
-      <c r="K60" s="51"/>
-      <c r="L60" s="51"/>
-      <c r="M60" s="51"/>
-      <c r="N60" s="51"/>
-      <c r="O60" s="48"/>
-      <c r="P60" s="49"/>
-      <c r="Q60" s="50"/>
+      <c r="A60" s="48"/>
+      <c r="B60" s="48"/>
+      <c r="C60" s="48"/>
+      <c r="D60" s="51"/>
+      <c r="E60" s="51"/>
+      <c r="F60" s="51"/>
+      <c r="G60" s="48"/>
+      <c r="H60" s="48"/>
+      <c r="I60" s="48"/>
+      <c r="J60" s="48"/>
+      <c r="K60" s="48"/>
+      <c r="L60" s="48"/>
+      <c r="M60" s="48"/>
+      <c r="N60" s="48"/>
+      <c r="O60" s="57"/>
+      <c r="P60" s="59"/>
+      <c r="Q60" s="60"/>
       <c r="R60" s="3"/>
       <c r="S60" s="3"/>
       <c r="T60" s="3"/>
@@ -31414,23 +31414,23 @@
       <c r="Z60" s="3"/>
     </row>
     <row r="61" spans="1:26" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A61" s="51"/>
-      <c r="B61" s="51"/>
-      <c r="C61" s="51"/>
-      <c r="D61" s="57"/>
-      <c r="E61" s="57"/>
-      <c r="F61" s="57"/>
-      <c r="G61" s="51"/>
-      <c r="H61" s="51"/>
-      <c r="I61" s="51"/>
-      <c r="J61" s="51"/>
-      <c r="K61" s="51"/>
-      <c r="L61" s="51"/>
-      <c r="M61" s="51"/>
-      <c r="N61" s="51"/>
-      <c r="O61" s="48"/>
-      <c r="P61" s="49"/>
-      <c r="Q61" s="50"/>
+      <c r="A61" s="48"/>
+      <c r="B61" s="48"/>
+      <c r="C61" s="48"/>
+      <c r="D61" s="51"/>
+      <c r="E61" s="51"/>
+      <c r="F61" s="51"/>
+      <c r="G61" s="48"/>
+      <c r="H61" s="48"/>
+      <c r="I61" s="48"/>
+      <c r="J61" s="48"/>
+      <c r="K61" s="48"/>
+      <c r="L61" s="48"/>
+      <c r="M61" s="48"/>
+      <c r="N61" s="48"/>
+      <c r="O61" s="57"/>
+      <c r="P61" s="59"/>
+      <c r="Q61" s="60"/>
       <c r="R61" s="3"/>
       <c r="S61" s="3"/>
       <c r="T61" s="3"/>
@@ -31442,39 +31442,39 @@
       <c r="Z61" s="3"/>
     </row>
     <row r="62" spans="1:26" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="58" t="s">
+      <c r="A62" s="47" t="s">
         <v>53</v>
       </c>
-      <c r="B62" s="55" t="s">
+      <c r="B62" s="49" t="s">
         <v>54</v>
       </c>
-      <c r="C62" s="51"/>
-      <c r="D62" s="56" t="s">
+      <c r="C62" s="48"/>
+      <c r="D62" s="50" t="s">
         <v>63</v>
       </c>
-      <c r="E62" s="57"/>
-      <c r="F62" s="57"/>
-      <c r="G62" s="53" t="s">
+      <c r="E62" s="51"/>
+      <c r="F62" s="51"/>
+      <c r="G62" s="52" t="s">
         <v>55</v>
       </c>
-      <c r="H62" s="51"/>
-      <c r="I62" s="51"/>
-      <c r="J62" s="49" t="s">
+      <c r="H62" s="48"/>
+      <c r="I62" s="48"/>
+      <c r="J62" s="59" t="s">
         <v>20</v>
       </c>
-      <c r="K62" s="51"/>
-      <c r="L62" s="51"/>
-      <c r="M62" s="54" t="s">
+      <c r="K62" s="48"/>
+      <c r="L62" s="48"/>
+      <c r="M62" s="53" t="s">
         <v>64</v>
       </c>
-      <c r="N62" s="51"/>
-      <c r="O62" s="47" t="s">
+      <c r="N62" s="48"/>
+      <c r="O62" s="56" t="s">
         <v>64</v>
       </c>
-      <c r="P62" s="49" t="s">
+      <c r="P62" s="59" t="s">
         <v>66</v>
       </c>
-      <c r="Q62" s="50"/>
+      <c r="Q62" s="60"/>
       <c r="R62" s="3"/>
       <c r="S62" s="3"/>
       <c r="T62" s="3"/>
@@ -31486,23 +31486,23 @@
       <c r="Z62" s="3"/>
     </row>
     <row r="63" spans="1:26" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A63" s="51"/>
-      <c r="B63" s="51"/>
-      <c r="C63" s="51"/>
-      <c r="D63" s="57"/>
-      <c r="E63" s="57"/>
-      <c r="F63" s="57"/>
-      <c r="G63" s="51"/>
-      <c r="H63" s="51"/>
-      <c r="I63" s="51"/>
-      <c r="J63" s="51"/>
-      <c r="K63" s="51"/>
-      <c r="L63" s="51"/>
-      <c r="M63" s="51"/>
-      <c r="N63" s="51"/>
-      <c r="O63" s="48"/>
-      <c r="P63" s="49"/>
-      <c r="Q63" s="50"/>
+      <c r="A63" s="48"/>
+      <c r="B63" s="48"/>
+      <c r="C63" s="48"/>
+      <c r="D63" s="51"/>
+      <c r="E63" s="51"/>
+      <c r="F63" s="51"/>
+      <c r="G63" s="48"/>
+      <c r="H63" s="48"/>
+      <c r="I63" s="48"/>
+      <c r="J63" s="48"/>
+      <c r="K63" s="48"/>
+      <c r="L63" s="48"/>
+      <c r="M63" s="48"/>
+      <c r="N63" s="48"/>
+      <c r="O63" s="57"/>
+      <c r="P63" s="59"/>
+      <c r="Q63" s="60"/>
       <c r="R63" s="3"/>
       <c r="S63" s="3"/>
       <c r="T63" s="3"/>
@@ -31514,23 +31514,23 @@
       <c r="Z63" s="3"/>
     </row>
     <row r="64" spans="1:26" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A64" s="51"/>
-      <c r="B64" s="51"/>
-      <c r="C64" s="51"/>
-      <c r="D64" s="57"/>
-      <c r="E64" s="57"/>
-      <c r="F64" s="57"/>
-      <c r="G64" s="51"/>
-      <c r="H64" s="51"/>
-      <c r="I64" s="51"/>
-      <c r="J64" s="51"/>
-      <c r="K64" s="51"/>
-      <c r="L64" s="51"/>
-      <c r="M64" s="51"/>
-      <c r="N64" s="51"/>
-      <c r="O64" s="48"/>
-      <c r="P64" s="49"/>
-      <c r="Q64" s="50"/>
+      <c r="A64" s="48"/>
+      <c r="B64" s="48"/>
+      <c r="C64" s="48"/>
+      <c r="D64" s="51"/>
+      <c r="E64" s="51"/>
+      <c r="F64" s="51"/>
+      <c r="G64" s="48"/>
+      <c r="H64" s="48"/>
+      <c r="I64" s="48"/>
+      <c r="J64" s="48"/>
+      <c r="K64" s="48"/>
+      <c r="L64" s="48"/>
+      <c r="M64" s="48"/>
+      <c r="N64" s="48"/>
+      <c r="O64" s="57"/>
+      <c r="P64" s="59"/>
+      <c r="Q64" s="60"/>
       <c r="R64" s="3"/>
       <c r="S64" s="3"/>
       <c r="T64" s="3"/>
@@ -31542,23 +31542,23 @@
       <c r="Z64" s="3"/>
     </row>
     <row r="65" spans="1:26" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A65" s="51"/>
-      <c r="B65" s="51"/>
-      <c r="C65" s="51"/>
-      <c r="D65" s="57"/>
-      <c r="E65" s="57"/>
-      <c r="F65" s="57"/>
-      <c r="G65" s="51"/>
-      <c r="H65" s="51"/>
-      <c r="I65" s="51"/>
-      <c r="J65" s="51"/>
-      <c r="K65" s="51"/>
-      <c r="L65" s="51"/>
-      <c r="M65" s="51"/>
-      <c r="N65" s="51"/>
-      <c r="O65" s="48"/>
-      <c r="P65" s="49"/>
-      <c r="Q65" s="50"/>
+      <c r="A65" s="48"/>
+      <c r="B65" s="48"/>
+      <c r="C65" s="48"/>
+      <c r="D65" s="51"/>
+      <c r="E65" s="51"/>
+      <c r="F65" s="51"/>
+      <c r="G65" s="48"/>
+      <c r="H65" s="48"/>
+      <c r="I65" s="48"/>
+      <c r="J65" s="48"/>
+      <c r="K65" s="48"/>
+      <c r="L65" s="48"/>
+      <c r="M65" s="48"/>
+      <c r="N65" s="48"/>
+      <c r="O65" s="57"/>
+      <c r="P65" s="59"/>
+      <c r="Q65" s="60"/>
       <c r="R65" s="3"/>
       <c r="S65" s="3"/>
       <c r="T65" s="3"/>
@@ -31570,23 +31570,23 @@
       <c r="Z65" s="3"/>
     </row>
     <row r="66" spans="1:26" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A66" s="51"/>
-      <c r="B66" s="51"/>
-      <c r="C66" s="51"/>
-      <c r="D66" s="57"/>
-      <c r="E66" s="57"/>
-      <c r="F66" s="57"/>
-      <c r="G66" s="51"/>
-      <c r="H66" s="51"/>
-      <c r="I66" s="51"/>
-      <c r="J66" s="51"/>
-      <c r="K66" s="51"/>
-      <c r="L66" s="51"/>
-      <c r="M66" s="51"/>
-      <c r="N66" s="51"/>
-      <c r="O66" s="48"/>
-      <c r="P66" s="49"/>
-      <c r="Q66" s="50"/>
+      <c r="A66" s="48"/>
+      <c r="B66" s="48"/>
+      <c r="C66" s="48"/>
+      <c r="D66" s="51"/>
+      <c r="E66" s="51"/>
+      <c r="F66" s="51"/>
+      <c r="G66" s="48"/>
+      <c r="H66" s="48"/>
+      <c r="I66" s="48"/>
+      <c r="J66" s="48"/>
+      <c r="K66" s="48"/>
+      <c r="L66" s="48"/>
+      <c r="M66" s="48"/>
+      <c r="N66" s="48"/>
+      <c r="O66" s="57"/>
+      <c r="P66" s="59"/>
+      <c r="Q66" s="60"/>
       <c r="R66" s="3"/>
       <c r="S66" s="3"/>
       <c r="T66" s="3"/>
@@ -31598,23 +31598,23 @@
       <c r="Z66" s="3"/>
     </row>
     <row r="67" spans="1:26" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A67" s="51"/>
-      <c r="B67" s="51"/>
-      <c r="C67" s="51"/>
-      <c r="D67" s="57"/>
-      <c r="E67" s="57"/>
-      <c r="F67" s="57"/>
-      <c r="G67" s="51"/>
-      <c r="H67" s="51"/>
-      <c r="I67" s="51"/>
-      <c r="J67" s="51"/>
-      <c r="K67" s="51"/>
-      <c r="L67" s="51"/>
-      <c r="M67" s="51"/>
-      <c r="N67" s="51"/>
-      <c r="O67" s="48"/>
-      <c r="P67" s="49"/>
-      <c r="Q67" s="50"/>
+      <c r="A67" s="48"/>
+      <c r="B67" s="48"/>
+      <c r="C67" s="48"/>
+      <c r="D67" s="51"/>
+      <c r="E67" s="51"/>
+      <c r="F67" s="51"/>
+      <c r="G67" s="48"/>
+      <c r="H67" s="48"/>
+      <c r="I67" s="48"/>
+      <c r="J67" s="48"/>
+      <c r="K67" s="48"/>
+      <c r="L67" s="48"/>
+      <c r="M67" s="48"/>
+      <c r="N67" s="48"/>
+      <c r="O67" s="57"/>
+      <c r="P67" s="59"/>
+      <c r="Q67" s="60"/>
       <c r="R67" s="3"/>
       <c r="S67" s="3"/>
       <c r="T67" s="3"/>
@@ -31626,39 +31626,39 @@
       <c r="Z67" s="3"/>
     </row>
     <row r="68" spans="1:26" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A68" s="58" t="s">
+      <c r="A68" s="47" t="s">
         <v>56</v>
       </c>
-      <c r="B68" s="53" t="s">
+      <c r="B68" s="52" t="s">
         <v>57</v>
       </c>
-      <c r="C68" s="51"/>
-      <c r="D68" s="56" t="s">
+      <c r="C68" s="48"/>
+      <c r="D68" s="50" t="s">
         <v>63</v>
       </c>
-      <c r="E68" s="57"/>
-      <c r="F68" s="57"/>
-      <c r="G68" s="53" t="s">
+      <c r="E68" s="51"/>
+      <c r="F68" s="51"/>
+      <c r="G68" s="52" t="s">
         <v>58</v>
       </c>
-      <c r="H68" s="51"/>
-      <c r="I68" s="51"/>
-      <c r="J68" s="49" t="s">
+      <c r="H68" s="48"/>
+      <c r="I68" s="48"/>
+      <c r="J68" s="59" t="s">
         <v>20</v>
       </c>
-      <c r="K68" s="51"/>
-      <c r="L68" s="51"/>
-      <c r="M68" s="47" t="s">
+      <c r="K68" s="48"/>
+      <c r="L68" s="48"/>
+      <c r="M68" s="56" t="s">
         <v>59</v>
       </c>
-      <c r="N68" s="52"/>
-      <c r="O68" s="47" t="s">
+      <c r="N68" s="58"/>
+      <c r="O68" s="56" t="s">
         <v>59</v>
       </c>
-      <c r="P68" s="49" t="s">
+      <c r="P68" s="59" t="s">
         <v>66</v>
       </c>
-      <c r="Q68" s="50"/>
+      <c r="Q68" s="60"/>
       <c r="R68" s="3"/>
       <c r="S68" s="3"/>
       <c r="T68" s="3"/>
@@ -31670,23 +31670,23 @@
       <c r="Z68" s="3"/>
     </row>
     <row r="69" spans="1:26" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A69" s="51"/>
-      <c r="B69" s="51"/>
-      <c r="C69" s="51"/>
-      <c r="D69" s="57"/>
-      <c r="E69" s="57"/>
-      <c r="F69" s="57"/>
-      <c r="G69" s="51"/>
-      <c r="H69" s="51"/>
-      <c r="I69" s="51"/>
-      <c r="J69" s="51"/>
-      <c r="K69" s="51"/>
-      <c r="L69" s="51"/>
-      <c r="M69" s="52"/>
-      <c r="N69" s="52"/>
-      <c r="O69" s="48"/>
-      <c r="P69" s="49"/>
-      <c r="Q69" s="50"/>
+      <c r="A69" s="48"/>
+      <c r="B69" s="48"/>
+      <c r="C69" s="48"/>
+      <c r="D69" s="51"/>
+      <c r="E69" s="51"/>
+      <c r="F69" s="51"/>
+      <c r="G69" s="48"/>
+      <c r="H69" s="48"/>
+      <c r="I69" s="48"/>
+      <c r="J69" s="48"/>
+      <c r="K69" s="48"/>
+      <c r="L69" s="48"/>
+      <c r="M69" s="58"/>
+      <c r="N69" s="58"/>
+      <c r="O69" s="57"/>
+      <c r="P69" s="59"/>
+      <c r="Q69" s="60"/>
       <c r="R69" s="3"/>
       <c r="S69" s="3"/>
       <c r="T69" s="3"/>
@@ -31698,23 +31698,23 @@
       <c r="Z69" s="3"/>
     </row>
     <row r="70" spans="1:26" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A70" s="51"/>
-      <c r="B70" s="51"/>
-      <c r="C70" s="51"/>
-      <c r="D70" s="57"/>
-      <c r="E70" s="57"/>
-      <c r="F70" s="57"/>
-      <c r="G70" s="51"/>
-      <c r="H70" s="51"/>
-      <c r="I70" s="51"/>
-      <c r="J70" s="51"/>
-      <c r="K70" s="51"/>
-      <c r="L70" s="51"/>
-      <c r="M70" s="52"/>
-      <c r="N70" s="52"/>
-      <c r="O70" s="48"/>
-      <c r="P70" s="49"/>
-      <c r="Q70" s="50"/>
+      <c r="A70" s="48"/>
+      <c r="B70" s="48"/>
+      <c r="C70" s="48"/>
+      <c r="D70" s="51"/>
+      <c r="E70" s="51"/>
+      <c r="F70" s="51"/>
+      <c r="G70" s="48"/>
+      <c r="H70" s="48"/>
+      <c r="I70" s="48"/>
+      <c r="J70" s="48"/>
+      <c r="K70" s="48"/>
+      <c r="L70" s="48"/>
+      <c r="M70" s="58"/>
+      <c r="N70" s="58"/>
+      <c r="O70" s="57"/>
+      <c r="P70" s="59"/>
+      <c r="Q70" s="60"/>
       <c r="R70" s="3"/>
       <c r="S70" s="3"/>
       <c r="T70" s="3"/>
@@ -31726,23 +31726,23 @@
       <c r="Z70" s="3"/>
     </row>
     <row r="71" spans="1:26" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A71" s="51"/>
-      <c r="B71" s="51"/>
-      <c r="C71" s="51"/>
-      <c r="D71" s="57"/>
-      <c r="E71" s="57"/>
-      <c r="F71" s="57"/>
-      <c r="G71" s="51"/>
-      <c r="H71" s="51"/>
-      <c r="I71" s="51"/>
-      <c r="J71" s="51"/>
-      <c r="K71" s="51"/>
-      <c r="L71" s="51"/>
-      <c r="M71" s="52"/>
-      <c r="N71" s="52"/>
-      <c r="O71" s="48"/>
-      <c r="P71" s="49"/>
-      <c r="Q71" s="50"/>
+      <c r="A71" s="48"/>
+      <c r="B71" s="48"/>
+      <c r="C71" s="48"/>
+      <c r="D71" s="51"/>
+      <c r="E71" s="51"/>
+      <c r="F71" s="51"/>
+      <c r="G71" s="48"/>
+      <c r="H71" s="48"/>
+      <c r="I71" s="48"/>
+      <c r="J71" s="48"/>
+      <c r="K71" s="48"/>
+      <c r="L71" s="48"/>
+      <c r="M71" s="58"/>
+      <c r="N71" s="58"/>
+      <c r="O71" s="57"/>
+      <c r="P71" s="59"/>
+      <c r="Q71" s="60"/>
       <c r="R71" s="3"/>
       <c r="S71" s="3"/>
       <c r="T71" s="3"/>
@@ -31754,23 +31754,23 @@
       <c r="Z71" s="3"/>
     </row>
     <row r="72" spans="1:26" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A72" s="51"/>
-      <c r="B72" s="51"/>
-      <c r="C72" s="51"/>
-      <c r="D72" s="57"/>
-      <c r="E72" s="57"/>
-      <c r="F72" s="57"/>
-      <c r="G72" s="51"/>
-      <c r="H72" s="51"/>
-      <c r="I72" s="51"/>
-      <c r="J72" s="51"/>
-      <c r="K72" s="51"/>
-      <c r="L72" s="51"/>
-      <c r="M72" s="52"/>
-      <c r="N72" s="52"/>
-      <c r="O72" s="48"/>
-      <c r="P72" s="49"/>
-      <c r="Q72" s="50"/>
+      <c r="A72" s="48"/>
+      <c r="B72" s="48"/>
+      <c r="C72" s="48"/>
+      <c r="D72" s="51"/>
+      <c r="E72" s="51"/>
+      <c r="F72" s="51"/>
+      <c r="G72" s="48"/>
+      <c r="H72" s="48"/>
+      <c r="I72" s="48"/>
+      <c r="J72" s="48"/>
+      <c r="K72" s="48"/>
+      <c r="L72" s="48"/>
+      <c r="M72" s="58"/>
+      <c r="N72" s="58"/>
+      <c r="O72" s="57"/>
+      <c r="P72" s="59"/>
+      <c r="Q72" s="60"/>
       <c r="R72" s="3"/>
       <c r="S72" s="3"/>
       <c r="T72" s="3"/>
@@ -31782,23 +31782,23 @@
       <c r="Z72" s="3"/>
     </row>
     <row r="73" spans="1:26" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A73" s="51"/>
-      <c r="B73" s="51"/>
-      <c r="C73" s="51"/>
-      <c r="D73" s="57"/>
-      <c r="E73" s="57"/>
-      <c r="F73" s="57"/>
-      <c r="G73" s="51"/>
-      <c r="H73" s="51"/>
-      <c r="I73" s="51"/>
-      <c r="J73" s="51"/>
-      <c r="K73" s="51"/>
-      <c r="L73" s="51"/>
-      <c r="M73" s="52"/>
-      <c r="N73" s="52"/>
-      <c r="O73" s="48"/>
-      <c r="P73" s="49"/>
-      <c r="Q73" s="50"/>
+      <c r="A73" s="48"/>
+      <c r="B73" s="48"/>
+      <c r="C73" s="48"/>
+      <c r="D73" s="51"/>
+      <c r="E73" s="51"/>
+      <c r="F73" s="51"/>
+      <c r="G73" s="48"/>
+      <c r="H73" s="48"/>
+      <c r="I73" s="48"/>
+      <c r="J73" s="48"/>
+      <c r="K73" s="48"/>
+      <c r="L73" s="48"/>
+      <c r="M73" s="58"/>
+      <c r="N73" s="58"/>
+      <c r="O73" s="57"/>
+      <c r="P73" s="59"/>
+      <c r="Q73" s="60"/>
       <c r="R73" s="3"/>
       <c r="S73" s="3"/>
       <c r="T73" s="3"/>
@@ -56871,20 +56871,81 @@
     </row>
   </sheetData>
   <mergeCells count="113">
-    <mergeCell ref="A62:A67"/>
-    <mergeCell ref="B62:C67"/>
-    <mergeCell ref="D62:F67"/>
-    <mergeCell ref="G62:I67"/>
-    <mergeCell ref="A68:A73"/>
-    <mergeCell ref="B68:C73"/>
-    <mergeCell ref="D68:F73"/>
-    <mergeCell ref="G68:I73"/>
-    <mergeCell ref="A44:A49"/>
-    <mergeCell ref="B44:C49"/>
-    <mergeCell ref="D44:F49"/>
-    <mergeCell ref="G44:I49"/>
-    <mergeCell ref="G50:I55"/>
-    <mergeCell ref="A50:A55"/>
+    <mergeCell ref="O62:O67"/>
+    <mergeCell ref="P62:P67"/>
+    <mergeCell ref="Q62:Q67"/>
+    <mergeCell ref="O68:O73"/>
+    <mergeCell ref="P68:P73"/>
+    <mergeCell ref="Q68:Q73"/>
+    <mergeCell ref="O50:O55"/>
+    <mergeCell ref="P50:P55"/>
+    <mergeCell ref="Q50:Q55"/>
+    <mergeCell ref="O56:O61"/>
+    <mergeCell ref="P56:P61"/>
+    <mergeCell ref="Q56:Q61"/>
+    <mergeCell ref="O38:O43"/>
+    <mergeCell ref="P38:P43"/>
+    <mergeCell ref="Q38:Q43"/>
+    <mergeCell ref="O44:O49"/>
+    <mergeCell ref="P44:P49"/>
+    <mergeCell ref="Q44:Q49"/>
+    <mergeCell ref="O26:O31"/>
+    <mergeCell ref="P26:P31"/>
+    <mergeCell ref="Q26:Q31"/>
+    <mergeCell ref="O32:O37"/>
+    <mergeCell ref="P32:P37"/>
+    <mergeCell ref="Q32:Q37"/>
+    <mergeCell ref="O14:O19"/>
+    <mergeCell ref="P14:P19"/>
+    <mergeCell ref="Q14:Q19"/>
+    <mergeCell ref="O20:O25"/>
+    <mergeCell ref="P20:P25"/>
+    <mergeCell ref="Q20:Q25"/>
+    <mergeCell ref="O2:O7"/>
+    <mergeCell ref="P2:P7"/>
+    <mergeCell ref="O8:O13"/>
+    <mergeCell ref="P8:P13"/>
+    <mergeCell ref="Q2:Q7"/>
+    <mergeCell ref="Q8:Q13"/>
+    <mergeCell ref="J62:L67"/>
+    <mergeCell ref="J68:L73"/>
+    <mergeCell ref="M68:N73"/>
+    <mergeCell ref="J44:L49"/>
+    <mergeCell ref="M44:N49"/>
+    <mergeCell ref="J50:L55"/>
+    <mergeCell ref="M50:N55"/>
+    <mergeCell ref="J56:L61"/>
+    <mergeCell ref="M56:N61"/>
+    <mergeCell ref="M62:N67"/>
+    <mergeCell ref="J32:L37"/>
+    <mergeCell ref="M32:N37"/>
+    <mergeCell ref="J38:L43"/>
+    <mergeCell ref="M38:N43"/>
+    <mergeCell ref="B50:C55"/>
+    <mergeCell ref="D50:F55"/>
+    <mergeCell ref="G26:I31"/>
+    <mergeCell ref="J2:L7"/>
+    <mergeCell ref="M2:N7"/>
+    <mergeCell ref="J8:L13"/>
+    <mergeCell ref="M8:N13"/>
+    <mergeCell ref="J14:L19"/>
+    <mergeCell ref="M14:N19"/>
+    <mergeCell ref="M20:N25"/>
+    <mergeCell ref="J20:L25"/>
+    <mergeCell ref="J26:L31"/>
+    <mergeCell ref="M26:N31"/>
+    <mergeCell ref="A20:A25"/>
+    <mergeCell ref="B20:C25"/>
+    <mergeCell ref="D20:F25"/>
+    <mergeCell ref="G20:I25"/>
+    <mergeCell ref="A2:A7"/>
+    <mergeCell ref="B2:C7"/>
+    <mergeCell ref="D2:F7"/>
+    <mergeCell ref="G2:I7"/>
+    <mergeCell ref="A8:A13"/>
+    <mergeCell ref="B8:C13"/>
+    <mergeCell ref="D8:F13"/>
+    <mergeCell ref="G8:I13"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="D1:F1"/>
     <mergeCell ref="G1:I1"/>
@@ -56909,81 +56970,20 @@
     <mergeCell ref="G14:I19"/>
     <mergeCell ref="B14:C19"/>
     <mergeCell ref="D14:F19"/>
-    <mergeCell ref="A20:A25"/>
-    <mergeCell ref="B20:C25"/>
-    <mergeCell ref="D20:F25"/>
-    <mergeCell ref="G20:I25"/>
-    <mergeCell ref="A2:A7"/>
-    <mergeCell ref="B2:C7"/>
-    <mergeCell ref="D2:F7"/>
-    <mergeCell ref="G2:I7"/>
-    <mergeCell ref="A8:A13"/>
-    <mergeCell ref="B8:C13"/>
-    <mergeCell ref="D8:F13"/>
-    <mergeCell ref="G8:I13"/>
-    <mergeCell ref="J32:L37"/>
-    <mergeCell ref="M32:N37"/>
-    <mergeCell ref="J38:L43"/>
-    <mergeCell ref="M38:N43"/>
-    <mergeCell ref="B50:C55"/>
-    <mergeCell ref="D50:F55"/>
-    <mergeCell ref="G26:I31"/>
-    <mergeCell ref="J2:L7"/>
-    <mergeCell ref="M2:N7"/>
-    <mergeCell ref="J8:L13"/>
-    <mergeCell ref="M8:N13"/>
-    <mergeCell ref="J14:L19"/>
-    <mergeCell ref="M14:N19"/>
-    <mergeCell ref="M20:N25"/>
-    <mergeCell ref="J20:L25"/>
-    <mergeCell ref="J26:L31"/>
-    <mergeCell ref="M26:N31"/>
-    <mergeCell ref="J62:L67"/>
-    <mergeCell ref="J68:L73"/>
-    <mergeCell ref="M68:N73"/>
-    <mergeCell ref="J44:L49"/>
-    <mergeCell ref="M44:N49"/>
-    <mergeCell ref="J50:L55"/>
-    <mergeCell ref="M50:N55"/>
-    <mergeCell ref="J56:L61"/>
-    <mergeCell ref="M56:N61"/>
-    <mergeCell ref="M62:N67"/>
-    <mergeCell ref="O14:O19"/>
-    <mergeCell ref="P14:P19"/>
-    <mergeCell ref="Q14:Q19"/>
-    <mergeCell ref="O20:O25"/>
-    <mergeCell ref="P20:P25"/>
-    <mergeCell ref="Q20:Q25"/>
-    <mergeCell ref="O2:O7"/>
-    <mergeCell ref="P2:P7"/>
-    <mergeCell ref="O8:O13"/>
-    <mergeCell ref="P8:P13"/>
-    <mergeCell ref="Q2:Q7"/>
-    <mergeCell ref="Q8:Q13"/>
-    <mergeCell ref="O38:O43"/>
-    <mergeCell ref="P38:P43"/>
-    <mergeCell ref="Q38:Q43"/>
-    <mergeCell ref="O44:O49"/>
-    <mergeCell ref="P44:P49"/>
-    <mergeCell ref="Q44:Q49"/>
-    <mergeCell ref="O26:O31"/>
-    <mergeCell ref="P26:P31"/>
-    <mergeCell ref="Q26:Q31"/>
-    <mergeCell ref="O32:O37"/>
-    <mergeCell ref="P32:P37"/>
-    <mergeCell ref="Q32:Q37"/>
-    <mergeCell ref="O62:O67"/>
-    <mergeCell ref="P62:P67"/>
-    <mergeCell ref="Q62:Q67"/>
-    <mergeCell ref="O68:O73"/>
-    <mergeCell ref="P68:P73"/>
-    <mergeCell ref="Q68:Q73"/>
-    <mergeCell ref="O50:O55"/>
-    <mergeCell ref="P50:P55"/>
-    <mergeCell ref="Q50:Q55"/>
-    <mergeCell ref="O56:O61"/>
-    <mergeCell ref="P56:P61"/>
-    <mergeCell ref="Q56:Q61"/>
+    <mergeCell ref="A62:A67"/>
+    <mergeCell ref="B62:C67"/>
+    <mergeCell ref="D62:F67"/>
+    <mergeCell ref="G62:I67"/>
+    <mergeCell ref="A68:A73"/>
+    <mergeCell ref="B68:C73"/>
+    <mergeCell ref="D68:F73"/>
+    <mergeCell ref="G68:I73"/>
+    <mergeCell ref="A44:A49"/>
+    <mergeCell ref="B44:C49"/>
+    <mergeCell ref="D44:F49"/>
+    <mergeCell ref="G44:I49"/>
+    <mergeCell ref="G50:I55"/>
+    <mergeCell ref="A50:A55"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>